<commit_message>
OOps forgot this boy
</commit_message>
<xml_diff>
--- a/Stimuli/MDMKChecker.xlsx
+++ b/Stimuli/MDMKChecker.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4500" uniqueCount="648">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4396" uniqueCount="653">
   <si>
     <t>y</t>
   </si>
@@ -1972,6 +1972,21 @@
   </si>
   <si>
     <t>Q2 Checker</t>
+  </si>
+  <si>
+    <t>The Kingsley Hills tourism board wants to build a___</t>
+  </si>
+  <si>
+    <t>The food festival is held___</t>
+  </si>
+  <si>
+    <t>Torton airfield is___</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Monument behind the summer lodges is to commemorate what? </t>
+  </si>
+  <si>
+    <t>The Ski resort caters to___</t>
   </si>
 </sst>
 </file>
@@ -2325,8 +2340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G53" sqref="G53"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2335,17 +2350,21 @@
       <c r="B1">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>364</v>
-      </c>
-      <c r="D1" t="s">
-        <v>283</v>
-      </c>
-      <c r="E1" t="s">
-        <v>365</v>
-      </c>
-      <c r="F1" t="s">
-        <v>366</v>
+      <c r="C1" t="str">
+        <f>C31</f>
+        <v>The old chapel relied on donations from the local community. The Alder family had donated a great deal of money to the chapel. However, it still wasn't enough to match the amount of money that the Dwight family had managed to raise for the chapel. However, a new property developer that had just moved in wanted to grease the wheels of his business plans and so started to spend generously in the village. When Mr.Roberts donated to the chapel, he donated more than the Alder Family.</v>
+      </c>
+      <c r="D1" t="str">
+        <f>E31</f>
+        <v>The old chapel relied on donations from the local community. The Alder family had donated a great deal of money to the chapel. However, it still wasn't enough to match the amount of money that the Dwight family had managed to raise for the chapel. However, a new property developer that had just moved in wanted to grease the wheels of his business plans and so started to spend generously in the village. When Mr.Roberts donated to the chapel he donated less than the Alder Family.</v>
+      </c>
+      <c r="E1" t="str">
+        <f>G31</f>
+        <v xml:space="preserve">The old chapel's doors stood wide open allowing full view of its interior. Inside there stood a magnificent, hundred year old altar. To the left of the alter stood the pulpit where the pastor would often hold his sermons from. A recent Archaeological discovery has led researchers to believe that there is a secret underground chamber somewhere to the left of the alter in the church. The local community considered the church an integral part of its identity, but the number of people attending had dwindled significantly over the past few years. </v>
+      </c>
+      <c r="F1" t="str">
+        <f>I31</f>
+        <v xml:space="preserve">The old chapel's doors stood wide open allowing full view of its interior. Inside there stood a magnificent, hundred year old altar. To the left of the alter stood the pulpit where the pastor would often hold his sermons from. A recent Archaeological discovery has led researchers to believe that there is a secret underground chamber somewhere to the right of the altar in the church. The local community considered the church an integral part of its identity, but the number of people attending had dwindled significantly over the past few years. </v>
       </c>
       <c r="G1">
         <v>1</v>
@@ -2447,17 +2466,21 @@
       <c r="B2">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
-        <v>367</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>287</v>
-      </c>
-      <c r="F2" t="s">
-        <v>286</v>
+      <c r="C2" t="str">
+        <f t="shared" ref="C2:C26" si="0">C32</f>
+        <v xml:space="preserve">Amy was a highly competent hiker and she loved to compete in time trials. She was annoyed at the fact that she hadn't managed to climb to the mountain's summit faster than Sam. The two were friends and their rivalry would spur them on to climbing faster and more dangerously in order to one up each other. Amy's friend Bradley wanted to impress her. When he climbed the mountain he gave it all he had and made sure that he was at least faster than Amy. The three loved to climb and loved nature so they always made sure to pick up their rubbish wherever they went. </v>
+      </c>
+      <c r="D2" t="str">
+        <f t="shared" ref="D2:D26" si="1">E32</f>
+        <v>Amy was a highly competent hiker and she loved to compete in time trials. She was annoyed at the fact that she hadn't managed to climb to the mountain's summit faster than Sam. The two were friends and their rivalry would spur them on to climbing faster and more dangerously in order to one up each other. Amy's friend Bradley wanted to impress her. When he climbed the mountain he gave it all he had but he simply wasn't as fast as Amy. The three loved to climb and loved nature so they always made sure to pick up their rubbish wherever they went.</v>
+      </c>
+      <c r="E2" t="str">
+        <f t="shared" ref="E2:E7" si="2">G32</f>
+        <v>The mountain stood proudly as it had done for thousands of years. People had always wanted to climb it so over the years a natural rest stop had developed above the camp at the mountain's base. The rest stop had over the years become popular with bird watchers. They had no interest in reaching the summit as it was the birds they came for. With a recent increase in tourism on the mountain there was a rumour that somewhere above the camp at the mountain's base there was a small area where people would go to throw their rubbish away.</v>
+      </c>
+      <c r="F2" t="str">
+        <f t="shared" ref="F2:F7" si="3">I32</f>
+        <v>The mountain stood proudly as it had done for thousands of years. People had always wanted to climb it so over the years a natural rest stop had developed above the camp at the mountain's base. The rest stop had over the years become popular with bird watchers. They had no interest in reaching the summit as it was the birds they came for. With a recent increase in tourism on the mountain there was a rumour that somewhere below the camp at the mountain's base there was a small area where people would go to throw their rubbish away.</v>
       </c>
       <c r="G2">
         <v>2</v>
@@ -2517,38 +2540,38 @@
         <v>11</v>
       </c>
       <c r="Z2" t="str">
-        <f t="shared" ref="Z2:AC26" si="0">I2</f>
+        <f t="shared" ref="Z2:AC26" si="4">I2</f>
         <v>A mountain ranger is at the rest stop which way does he need to go to find where tourists throw their rubbish?</v>
       </c>
       <c r="AA2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>Up the mountain</v>
       </c>
       <c r="AB2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> Down the mountain</v>
       </c>
       <c r="AC2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>There is not enough information</v>
       </c>
       <c r="AD2">
         <v>2</v>
       </c>
       <c r="AE2" t="str">
-        <f t="shared" ref="AE2:AH26" si="1">N2</f>
+        <f t="shared" ref="AE2:AH26" si="5">N2</f>
         <v>Every year there is a race to the top of the mountain which allows only the best to compete, who is most likely to qualify?</v>
       </c>
       <c r="AF2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">Bradley </v>
       </c>
       <c r="AG2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Sam</v>
       </c>
       <c r="AH2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>There is not enough information</v>
       </c>
       <c r="AI2">
@@ -2559,17 +2582,21 @@
       <c r="B3">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
-        <v>368</v>
-      </c>
-      <c r="D3" t="s">
-        <v>288</v>
-      </c>
-      <c r="E3" t="s">
-        <v>369</v>
-      </c>
-      <c r="F3" t="s">
-        <v>370</v>
+      <c r="C3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">The town surgery had three resident GPs. Malcom who had been at the surgery the longest was liked well enough by the people who came to the surgery but his popularity was overshadowed by Sue who was very well liked by patients. With the surgery's refurbishment came a third GP, Matthew, whose kind nature made him very popular with the townsfolk, more popular than at Malcom. It didn't matter to them though as their main goal was to provide the best medical care they could to help their community. </v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" si="1"/>
+        <v>The town surgery had three resident GPs. Malcom who had been at the surgery the longest was liked well enough by the people who came to the surgery but his popularity was overshadowed by Sue who was very well liked by patients. With the surgery's refurbishment came a third GP, Matthew, whose kind nature made him very popular with the townsfolk, but not as popular as Malcom. It didn't matter to them though as their main goal was to provide the best medical care they could to help their community.</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">The newly refurbished town surgery was finally ready to reopen after a whole month of being closed. The surgery was located in front of a small play park surrounded by a large car park that was used for local shopping. The surgery boasted more space than it had before, several smaller buildings around were now used to house non-medical tools like cleaning equipment. The cleaner would keep his floor polisher in a shed somewhere behind the surgery. The cleaner had worked at the surgery for as long as anyone could remember. </v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">The newly refurbished town surgery was finally ready to reopen after a whole month of being closed. The surgery was located in front of a small play park surrounded by a large car park that was used for local shopping. The surgery boasted more space than it had before, several smaller buildings around were now used to house non-medical tools like cleaning equipment. The cleaner would keep his floor polisher in a shed somewhere in front of the surgery. The cleaner had worked at the surgery for as long as anyone could remember. </v>
       </c>
       <c r="G3">
         <v>3</v>
@@ -2629,38 +2656,38 @@
         <v>11</v>
       </c>
       <c r="Z3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>The cleaner is standing in the small play park facing away from the surgery, which way does he need to go to pick up his floor polisher from the shed?</v>
       </c>
       <c r="AA3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>Forward</v>
       </c>
       <c r="AB3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>Backward</v>
       </c>
       <c r="AC3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>There is not enough information</v>
       </c>
       <c r="AD3">
         <v>2</v>
       </c>
       <c r="AE3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Patients have voted for their favourite GP, who is likely to be the most popular?</v>
       </c>
       <c r="AF3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Malcom</v>
       </c>
       <c r="AG3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Sue</v>
       </c>
       <c r="AH3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>There is not enough information</v>
       </c>
       <c r="AI3">
@@ -2671,17 +2698,21 @@
       <c r="B4">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
-        <v>371</v>
-      </c>
-      <c r="D4" t="s">
-        <v>372</v>
-      </c>
-      <c r="E4" t="s">
-        <v>292</v>
-      </c>
-      <c r="F4" t="s">
-        <v>293</v>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Benjamin, the mechanic, had only just arrived on the island. He had been called there on the behest of his friend Allan, who was also a mechanic, to fix the island's lighthouse. Benjamin was not as good of a mechanic as Allan. After a long day of trying to repair the lighthouse there was still much work to do to get it working. Allan decided to call for help. Susan, who also lived on the Island, was not as good of a mechanic as Allan but surely the three of them would complete the work faster than just the two of them. </v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Benjamin, the mechanic, had only just arrived on the island. He had been called there on the behest of his friend Allan, who was also a mechanic, to fix the island's lighthouse. Benjamin was not as good of a mechanic as Allan. After a long day of trying to repair the lighthouse there was still much work to do to get it working. Allan decided to call for help. Susan, who also lived on the Island, was a better mechanic than Allan and surely the three of them would complete the work faster than just the two of them. </v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="2"/>
+        <v>Spice Island lay just three miles off shore. The island didn't have a lot to offer in terms of comfort but there were a handful of people that called it home. There was a small weather station to the left the small docks used mostly to load and unload supplies as well as passengers. There was also a supply store somewhere to the left of the docks. It was overpriced due to the fact that spice islanders had to import everything from the mainland. Many of them didn't mind spending more on supplies if it meant avoiding a long trip to the mainland.</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="3"/>
+        <v>Spice Island lay just three miles off shore. The island didn't have a lot to offer in terms of comfort but there were a handful of people that called it home. There was a small weather station to the left the small docks used mostly to load and unload supplies as well as passengers. There was also a supply store somewhere to the right of the docks. It was overpriced due to the fact that spice islanders had to import everything from the mainland. Many of them didn't mind spending more on supplies if it meant avoiding a long trip to the mainland.</v>
       </c>
       <c r="G4">
         <v>4</v>
@@ -2741,38 +2772,38 @@
         <v>11</v>
       </c>
       <c r="Z4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>Allan is standing in front of the weather station facing it, in which direction does he need to go to get to the shop?</v>
       </c>
       <c r="AA4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>Left</v>
       </c>
       <c r="AB4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>Right</v>
       </c>
       <c r="AC4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>There is not enough information</v>
       </c>
       <c r="AD4">
         <v>2</v>
       </c>
       <c r="AE4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">The least skilled mechanic is sent to pick up some coffee, who is this likely to be? </v>
       </c>
       <c r="AF4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Susan</v>
       </c>
       <c r="AG4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">Benjamin </v>
       </c>
       <c r="AH4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>There is not enough information</v>
       </c>
       <c r="AI4">
@@ -2783,17 +2814,21 @@
       <c r="B5">
         <v>5</v>
       </c>
-      <c r="C5" t="s">
-        <v>373</v>
-      </c>
-      <c r="D5" t="s">
-        <v>298</v>
-      </c>
-      <c r="E5" t="s">
-        <v>374</v>
-      </c>
-      <c r="F5" t="s">
-        <v>375</v>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Terrance had loved caving ever since he was introduced to it by his mother, Joan. Though she was getting older now she was still more experienced than him. The two would often plan family vacations that just happened to be in the vicinity of safe but challenging cave systems. Terrance's father had left before he was born, so when his mother had married his stepfather Stephen, Terrance was excited about the family holidays they could go on now as a trio. Stephen had an adventurous streak and also loved caving, though he was also not as experienced as Joan. </v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="1"/>
+        <v>Terrance had loved caving ever since he was introduced to it by his mother, Joan. Though she was getting older now she was still more experienced than him. The two would often plan family vacations that just happened to be in the vicinity of safe but challenging cave systems. Terrance's father had left before he was born, so when his mother had married his stepfather Stephen, Terrance was excited about the family holidays they could go on now as a trio. Stephen had an adventurous streak and also loved caving, and he was a far more experienced caver than Joan.</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">The locals had long considered the caves at the bottom of the Lincoln gorge dangerous. However, the tourist industry just kept growing. An adventure holiday company had set up a rest stop in a cave somewhere below the largest cavern. The largest cavern was usually the only place inexperienced cavers got to before turning back as the tunnel that went further was a very tight squeeze. A recent geological survey of the area had determined that there should be a previously undiscovered cavern somewhere below the largest cavern. </v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">The locals had long considered the caves at the bottom of the Lincoln gorge dangerous. However, the tourist industry just kept growing. An adventure holiday company had set up a rest stop in a cave somewhere below the largest cavern. The largest cavern was usually the only place inexperienced cavers got to before turning back as the tunnel that went further was a very tight squeeze. A recent geological survey of the area had determined that there should be a previously undiscovered cavern somewhere above the largest cavern. </v>
       </c>
       <c r="G5">
         <v>5</v>
@@ -2853,38 +2888,38 @@
         <v>11</v>
       </c>
       <c r="Z5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>In which general direction would Joan need to go to find the undiscovered cavern if she started at the rest stop?</v>
       </c>
       <c r="AA5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>Up</v>
       </c>
       <c r="AB5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>Down</v>
       </c>
       <c r="AC5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>There is not enough information</v>
       </c>
       <c r="AD5">
         <v>1</v>
       </c>
       <c r="AE5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>The least experienced caver in Terrance's family is made to pack lunch, who is this likely to be?</v>
       </c>
       <c r="AF5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Terrance</v>
       </c>
       <c r="AG5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Stephen</v>
       </c>
       <c r="AH5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>There is not enough information</v>
       </c>
       <c r="AI5">
@@ -2895,17 +2930,21 @@
       <c r="B6">
         <v>6</v>
       </c>
-      <c r="C6" t="s">
-        <v>376</v>
-      </c>
-      <c r="D6" t="s">
-        <v>377</v>
-      </c>
-      <c r="E6" t="s">
-        <v>378</v>
-      </c>
-      <c r="F6" t="s">
-        <v>379</v>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Harriet often travelled the long A67 highway. She had what she considered to be one of the most expensive cars in her neighbourhood, far more expensive than her neighbour Barry's car. Harriet was arrogant and boastful so it made her happy that he struggled to purchase his car whereas she could easily afford hers. Harriet's other neighbour Olive had a much nicer and more expensive car than Barry. Harriet enjoyed washing her car every weekend. </v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Harriet often travelled the long A67 highway. She had what she considered to be one of the most expensive cars in her neighbourhood, far more expensive than her neighbour Barry's car. Harriet was arrogant and boastful so it made her happy that he struggled to purchase his car whereas she could easily afford hers. Harriet's other neighbour Olive had an even less expensive car than Barry. Harriet enjoyed washing her car every weekend. </v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">The A67 highway was the longest road in the county. It spanned almost all of it, and ran over the river Stig. Heading to Innsmouth from Ipswich people had to cross the bridge over the river. Somewhere before this bridge there was a rest stop that offered travellers refreshment. It was a popular place and saw a great many visitors, making it a profitable place to own. A checkpoint had been set up by the police somewhere after the rest stop as there had been reports of drug smuggling in the area. </v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">The A67 highway the longest road in the county. It spanned almost all of it, and ran over the river Stig. Heading to Innsmouth from Ipswich people had to cross the bridge over the river. Somewhere before this bridge there was a rest stop that offered travellers refreshment. It was a popular place and saw a great many visitors, making it a profitable place to own. A checkpoint had been set up by the police somewhere before the rest stop as there had been reports of drug smuggling in the area. </v>
       </c>
       <c r="G6">
         <v>6</v>
@@ -2965,38 +3004,38 @@
         <v>11</v>
       </c>
       <c r="Z6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>Harriet is on the bridge heading for the rest stop, which way would she need to go if she wanted to see the the police check point?</v>
       </c>
       <c r="AA6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>Back</v>
       </c>
       <c r="AB6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>Ahead</v>
       </c>
       <c r="AC6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>There is not enough information</v>
       </c>
       <c r="AD6">
         <v>1</v>
       </c>
       <c r="AE6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">A burgalar is going to steal the most expensive car in the neighbourhood, who's car is most likely to be stolen? </v>
       </c>
       <c r="AF6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Harriet's</v>
       </c>
       <c r="AG6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Olive's</v>
       </c>
       <c r="AH6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>There is not enough information</v>
       </c>
       <c r="AI6">
@@ -3007,17 +3046,21 @@
       <c r="B7">
         <v>7</v>
       </c>
-      <c r="C7" t="s">
-        <v>380</v>
-      </c>
-      <c r="D7" t="s">
-        <v>381</v>
-      </c>
-      <c r="E7" t="s">
-        <v>302</v>
-      </c>
-      <c r="F7" t="s">
-        <v>303</v>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>Sunnydale high school was like any high school. The basketball group was quite popular even more popular than the football group. This may have been down to their recent win streak against their rival high school, which had put them on their way to the basketball finals. On another hand the art club had recently also exploded in popularity due to their very successful summer exhibition. Though they were still less popular than the basketball group. Their popularity would influence how many members each group had</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="1"/>
+        <v>Sunnydale high school was like any high school. The basketball group was quite popular even more popular than the football group. This may have been down to their recent win streak against their rival high school, which had put them on their way to the basketball finals. On another hand the art club had recently also exploded in popularity due to their very successful summer exhibition. It was apparent that their popularity had surpassed that of the basketball group.Their popularity would influence how many members each group had.</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="2"/>
+        <v>The hall had been rented out for the high school's prom. The theme was 1950's and the hall had been decorated accordingly with bunting and posters from the era. To the right of the table with snacks and refreshments stood a photo booth, where students could have their pictures taken in their fancy dress consumes. Somewhere to the left of the photo booth stood a table where students could write their well wishes to their fellow students, teachers, parents or anyone that had helped them get through the year. All the tickets for the prom had sold out almost immediately.</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="3"/>
+        <v>The hall had been rented out for the high school's prom. The theme was 1950's and the hall had been decorated accordingly with bunting and posters from the era. To the right of the table with snacks and refreshments stood a photo booth, where students could have their pictures taken in their fancy dress consumes. To the right of the photo booth stood a table where students could write their well wishes to their fellow students, teachers, parents or anyone that had helped them get through the year. All the tickets for the prom had sold out almost immediately.</v>
       </c>
       <c r="G7">
         <v>7</v>
@@ -3077,38 +3120,38 @@
         <v>11</v>
       </c>
       <c r="Z7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>Which way would one have to go in order to get from the refreshments table to the table with well wishes?</v>
       </c>
       <c r="AA7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>Left</v>
       </c>
       <c r="AB7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>Right</v>
       </c>
       <c r="AC7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>There is not enough information</v>
       </c>
       <c r="AD7">
         <v>2</v>
       </c>
       <c r="AE7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">Based on their popularity, which of the groups should have the fewest members? </v>
       </c>
       <c r="AF7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">The football team </v>
       </c>
       <c r="AG7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>The art club</v>
       </c>
       <c r="AH7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>There is not enough information</v>
       </c>
       <c r="AI7">
@@ -3119,17 +3162,21 @@
       <c r="B8">
         <v>8</v>
       </c>
-      <c r="C8" t="s">
-        <v>382</v>
-      </c>
-      <c r="D8" t="s">
-        <v>356</v>
-      </c>
-      <c r="E8" t="s">
-        <v>383</v>
-      </c>
-      <c r="F8" t="s">
-        <v>384</v>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">The Dunwich marathon drew from all over the county. Mike and his two friends, Ralph and Dustin, had come from two towns over to participate. Mike knew that he wasn't as good of a runner as Ralph. Dustin was a relatively new friend of theirs having only joined their company a few months ago, but they absolutely loved him. As soon as the marathon began it became apparent that Dustin, like Ralph was a much better runner than Mike. This was going to be another tough one for Mike. </v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="1"/>
+        <v>The Dunwich marathon drew runners from all over the county. Mike and his two friends, Ralph and Dustin, had come from two towns over to participate. Mike knew that he wasn't as good of a runner as Ralph. Dustin was a relatively new friend of theirs having only joined their company a few months ago, but they absolutely loved him. As soon as the marathon began it became apparent that Dustin, unlike Ralph wasn't a better runner than Mike. This was still going to be another tough one for Mike.</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" ref="E8:E26" si="6">G38</f>
+        <v>The marathon was held every year in Dunwich. All runners ran for a charity of their chosing and would run in a group together in order to stand out more for the crowds that gathered along the roads. The runners of the local hospice knew they were behind the runners of the wildlife charity. It didn't matter who won of course so long as everyone had fun. The runners from the cancer charity knew they were in front of the runners from the hospice, which encouraged them. It would be a spectacular finish with a great deal of money raised for charity.</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" ref="F8:F26" si="7">I38</f>
+        <v>The marathon was held every year in Dunwich. All runners ran for a charity of their chosing and would run in a group together in order to stand out more for the crowds that gathered along the roads. The runners of the local hospice knew they were behind the runners of the wildlife charity. It didn't matter who won of course so long as everyone had fun. The runners from the cancer charity knew they were behind of the runners from the hospice, which encouraged them. It would be a spectacular finish with a great deal of money raised for charity.</v>
       </c>
       <c r="G8">
         <v>8</v>
@@ -3189,38 +3236,38 @@
         <v>11</v>
       </c>
       <c r="Z8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>Which of the chairty running teams is most likely to finish the marathon first?</v>
       </c>
       <c r="AA8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">The wildlife charity </v>
       </c>
       <c r="AB8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">The cancer charity </v>
       </c>
       <c r="AC8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>There is not enough information</v>
       </c>
       <c r="AD8">
         <v>1</v>
       </c>
       <c r="AE8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>After the marathon the three friends decide to compete against each other, who is most likely to win?</v>
       </c>
       <c r="AF8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Dustin</v>
       </c>
       <c r="AG8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">Ralph </v>
       </c>
       <c r="AH8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>There is not enough information</v>
       </c>
       <c r="AI8">
@@ -3231,17 +3278,21 @@
       <c r="B9">
         <v>9</v>
       </c>
-      <c r="C9" t="s">
-        <v>385</v>
-      </c>
-      <c r="D9" t="s">
-        <v>386</v>
-      </c>
-      <c r="E9" t="s">
-        <v>387</v>
-      </c>
-      <c r="F9" t="s">
-        <v>388</v>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Jonathan had been looking forward to his skiing trip for a while now. Recent profitable returns on some risky investments had made him a lot of money and it was time to flaunt it. He knew that his university rival, Thom, would be skiing at the same resort as him and it made him very happy to know that his net worth was now, way above Thom's. Jonathan had invited his childhood friend Catherine to go skiing with him. Catherine had been born very wealthy but not as wealthy as Jonathan. </v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Jonathan had been looking forward to his skiing trip for a while now. Recent profitable returns on some risky investments had made him a lot of money and it was time to flaunt it. He knew that his university rival, Thom, would be skiing at the same resort as him and it made him very happy to know that his net worth was now, way above Thom's. Jonathan had invited his childhood friend Catherine to go skiing with him. Catherine had been born rich and was even wealthier than Jonathan. </v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">High up in the mountains, is a world famous ski resort. The resort caters almost exclusively to the incredibly wealthy. It has some of the finest hotels and restaurants in the world. The slope everyone at the resort desired to be seen on was above the most exclusive ski lodge. People had to be specially invited to stay at the lodge. Though the lodge couldn't actually stop anyone from skiing on the slope, they were responsible for its upkeep and safety. A child has gone missing somewhere below the start of the slope and hadn't been seen in several hours. </v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">High up in the mountains, is a world famous ski resort. The resort caters almost exclusively to the incredibly wealthy. It has some of the finest hotels and restaurants in the world. The slope everyone at the resort desired to be seen on was above the most exclusive ski lodge. People had to be specially invited to stay at the lodge.Though the lodge couldn't actually stop anyone from skiing on the slope, they were responsible for its upkeep and safety. A child has gone missing somewhere above the start of the slope and hadn't been seen in several hours. </v>
       </c>
       <c r="G9">
         <v>9</v>
@@ -3280,7 +3331,7 @@
         <v>3</v>
       </c>
       <c r="S9" t="s">
-        <v>82</v>
+        <v>652</v>
       </c>
       <c r="T9" t="s">
         <v>83</v>
@@ -3301,38 +3352,38 @@
         <v>11</v>
       </c>
       <c r="Z9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">The Lodge staff are leaving the Lodge to look for the missing child, which way should they head? </v>
       </c>
       <c r="AA9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>Upward</v>
       </c>
       <c r="AB9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>Downward</v>
       </c>
       <c r="AC9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>There is not enough information</v>
       </c>
       <c r="AD9">
         <v>1</v>
       </c>
       <c r="AE9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Jonathan, Catherine and Thom are the first to arrive at the lodge this season, who is the least wealthy out of all of them?</v>
       </c>
       <c r="AF9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Catherine</v>
       </c>
       <c r="AG9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">Thom </v>
       </c>
       <c r="AH9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>There is not enough information</v>
       </c>
       <c r="AI9">
@@ -3343,17 +3394,21 @@
       <c r="B10">
         <v>10</v>
       </c>
-      <c r="C10" t="s">
-        <v>389</v>
-      </c>
-      <c r="D10" t="s">
-        <v>86</v>
-      </c>
-      <c r="E10" t="s">
-        <v>390</v>
-      </c>
-      <c r="F10" t="s">
-        <v>308</v>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Agatha was a spectacular horticulturalist. She was better even than Sam who owned the flower shop. If there was something that Sam didn't know or wasn't sure about it was Agatha that she would go to. The two had worked together on multiple projects in the past. Recently a new flower shop had opened up in the next town over, its proprietor was none other than Sam's old rival Rachel who was much more knowledgeable than Sam when it came to Flowers. </v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="1"/>
+        <v>Agatha was a spectacular horticulturalist. She was better even than Sam who owned the flower shop. If there was something that Sam didn't know or wasn't sure about it was Agatha that she would go to. The two had worked together on multiple projects in the past. Recently a new flower shop had opened up in the next town over, its proprietor was none other than Sam's old rival Rachel who wasn't as knowledgeable as Sam when it came to Flowers.</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">The flower shop on Wensley High Street was the town's favourite. To the right of display of pre-cut flowers was an arrangement of succulents that would change every week. It was one of the reasons why the shop was so popular, people loved the fact that they could return weekly and find something new. Recently a local prankster had taken to putting fake plastic plants with price tags somewhere to the right of the cut flowers, much to the dismay of anyone unfortunate enough to accidentally purchase them. </v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="7"/>
+        <v>The flower shop on Wensley High Street was the town's favourite. To the right of display of pre-cut flowers was an arrangement of succulents that would change every week. It was one of the reasons why the shop was so popular, people loved the fact that they could return weekly and find something new. Recently a local prankster had taken to putting fake plastic plants with price tags somewhere to the left of the cut flowers, much to the dismay of anyone unfortunate enough to accidentally purchase them.</v>
       </c>
       <c r="G10">
         <v>10</v>
@@ -3413,38 +3468,38 @@
         <v>11</v>
       </c>
       <c r="Z10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>Sam wants to get rid of the plastic plants. She is standing in front of the succulents in which direction should she look to find the plastic plants?</v>
       </c>
       <c r="AA10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>Right</v>
       </c>
       <c r="AB10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">Left </v>
       </c>
       <c r="AC10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>There is not enough information</v>
       </c>
       <c r="AD10">
         <v>2</v>
       </c>
       <c r="AE10" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">A prize is given every year to the most skilled horticulturalist, who is most likely to win? </v>
       </c>
       <c r="AF10" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Agatha</v>
       </c>
       <c r="AG10" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Rachel</v>
       </c>
       <c r="AH10" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>There is not enough information</v>
       </c>
       <c r="AI10">
@@ -3455,17 +3510,21 @@
       <c r="B11">
         <v>11</v>
       </c>
-      <c r="C11" t="s">
-        <v>391</v>
-      </c>
-      <c r="D11" t="s">
-        <v>392</v>
-      </c>
-      <c r="E11" t="s">
-        <v>393</v>
-      </c>
-      <c r="F11" t="s">
-        <v>394</v>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Peter, Sally and Joanna were best of friends. They Loved to play together. Their parents didn't like the three playing together, they were far more concerned as to what people thought about them. Joanna's family wasn't as well respected as Peter's due to Joanna's brother turning to crime a few years ago and going to prison. Sally's family was also not as well respected as Peter's family. However, none of this ever bothered the three at all. No matter what was done or said to them they always found a way to spend the entire summer together. </v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Peter, Sally and Joanna were best of friends.They Loved to play together. Their parents didn't like the three playing together, they were far more concerned as to what people thought about them. Joanna's family wasn't as well respected as Peter's due to Joanna's brother turning to crime a few years ago and going to prison. Though Sally's family was far more respected than Peter's family. However, none of this ever bothered the three at all. No matter what was done or said to them they always found a way to spend the entire summer together. </v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">The village of Northport didn't offer that much in terms of regular amusement but it had some of the best camping around. Behind the rows of summer lodges was a stream where kids from the village would spend their entire summer. They often played with those that had come to Northport for the camping. Many friendships were forged in and around that stream. Behind the summer lodges stood a monument to a dog that had saved his owners life during a bear attack at the cost of its own. </v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">The village of Northport didn't offer that much in terms of regular amusement but it had some of the best camping around. Behind the rows of summer lodges was a stream where kids from the village would spend their entire summer. They often played with those that had come to Northport for the camping. Many friendships were forged in and around that stream. In front of the summer lodges stood a monument to a dog that had saved his owners life during a bear attack at the cost of its own. </v>
       </c>
       <c r="G11">
         <v>11</v>
@@ -3504,7 +3563,7 @@
         <v>3</v>
       </c>
       <c r="S11" t="s">
-        <v>101</v>
+        <v>651</v>
       </c>
       <c r="T11" t="s">
         <v>102</v>
@@ -3525,38 +3584,38 @@
         <v>11</v>
       </c>
       <c r="Z11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">A holiday maker has lost his watch by the monument, he is standing by the stream. Which general direction should he head to find his watch ? </v>
       </c>
       <c r="AA11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>Ahead, away from the Lodges</v>
       </c>
       <c r="AB11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>Back, towards the Lodges</v>
       </c>
       <c r="AC11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>There is not enough information</v>
       </c>
       <c r="AD11">
         <v>2</v>
       </c>
       <c r="AE11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">A new family has moved into town and tells their son to stay away from the least respected family. Which family is this likely to be? </v>
       </c>
       <c r="AF11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Sally's</v>
       </c>
       <c r="AG11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Joanna's</v>
       </c>
       <c r="AH11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>There is not enough information</v>
       </c>
       <c r="AI11">
@@ -3567,17 +3626,21 @@
       <c r="B12">
         <v>12</v>
       </c>
-      <c r="C12" t="s">
-        <v>395</v>
-      </c>
-      <c r="D12" t="s">
-        <v>105</v>
-      </c>
-      <c r="E12" t="s">
-        <v>396</v>
-      </c>
-      <c r="F12" t="s">
-        <v>397</v>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Terry was one of the most experienced pilots in Torton, he'd been flying since he was a boy, he was in fact a far more experienced pilot than Josh who had been managing Torton Airfield for several years now. The two got along fantastically and would often go for drinks together at the pub. This year a new pilot had arrived in Torton, Aaron, an ex-stunt pilot who became a flight instructor. Aaron had a great deal more experience than Josh. </v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="1"/>
+        <v>Terry was one of the most experienced pilots in Torton, he'd been flying since he was a boy, he was in fact a far more experienced pilot than Josh who had been managing Torton Airfield for several years now. The two got along fantastically and would often go for drinks together at the pub. This year a new pilot had arrived in Torton, Aaron, an ex-stunt pilot who became a flight instructor. Aaron was not more experienced than Josh.</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">The Torton airfield was busy this time of year. The resident helicopter flight instructor was flying somewhere above the control tower. He liked to tease the people in the control tower with stunts looked like they would end in a crash. The tower couldn't care less though. They were dealing with a landing request from a small biplane that was having a few engine troubles but it was high above them so it had plenty of space and speed to be able to make a safe landing. </v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">The Torton airfield was busy this time of year. The resident helicopter flight instructor was flying somewhere above the control tower. He liked to tease the people in the control tower with stunts looked like they would end in a crash. The tower couldn't care less though. They were dealing with a take-off request from a small biplane that was having a few engine troubles that morning. The tower wasn't sure if the mechanic had resolved the issue so at this point the tower could not OK the take off. </v>
       </c>
       <c r="G12">
         <v>12</v>
@@ -3616,7 +3679,7 @@
         <v>3</v>
       </c>
       <c r="S12" t="s">
-        <v>112</v>
+        <v>650</v>
       </c>
       <c r="T12" t="s">
         <v>113</v>
@@ -3637,38 +3700,38 @@
         <v>11</v>
       </c>
       <c r="Z12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>The helicopter pilot wants to know if he is flying higher than the biplane. Which aircraft is higher?</v>
       </c>
       <c r="AA12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>The Helicopter</v>
       </c>
       <c r="AB12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">The Biplane </v>
       </c>
       <c r="AC12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>There is not enough information</v>
       </c>
       <c r="AD12">
         <v>1</v>
       </c>
       <c r="AE12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Next year Taunton airfield will host a small air show, who is the most experienced pilot ?</v>
       </c>
       <c r="AF12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Josh</v>
       </c>
       <c r="AG12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Terry</v>
       </c>
       <c r="AH12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>There is not enough information</v>
       </c>
       <c r="AI12">
@@ -3679,17 +3742,21 @@
       <c r="B13">
         <v>13</v>
       </c>
-      <c r="C13" t="s">
-        <v>359</v>
-      </c>
-      <c r="D13" t="s">
-        <v>398</v>
-      </c>
-      <c r="E13" t="s">
-        <v>399</v>
-      </c>
-      <c r="F13" t="s">
-        <v>312</v>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>The office workers had decided to organise a barbeque. The local beach would be the perfect place to set up. The only thing left was deciding who would be in charge of the grill. Everyone knew David was a better cook than Felix. It would be a big responsibility to ensure that the fine quality meats which had been ordered were cooked to perfection. A recent arrival at the office, Ella, had previously worked in agriculture and was considered to be not as good a cook as David.</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">The office workers had decided to organise a barbeque. The local beach would be the perfect place to set up. The only thing left was deciding who would be in charge of the grill. Everyone knew David was a better cook than Felix. It would be a big responsibility to ensure that the fine quality meats which had been ordered were cooked to perfection. A recent arrival at the office, Ella, had previously worked in agriculture and was considered a much better cook than David. </v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">The office was always busy this time of year. Somewhere to the left of the office managers desk stood a water cooler. She had placed it there so that she could keep an eye on her underlings so that they wouldn't be tempted to chat away the whole working day. The air conditioner had broken making the office hellishly hot. The manager had placed an order for a large fan so that it would be cooler. She'd made sure that it would be placed somewhere to the right of the watercooler so that she could keep an eye on it and control the settings if she needed to. </v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="7"/>
+        <v>The office was always busy this time of year. Somewhere to the left of the office managers desk stood a water cooler. She had placed it there so that she could keep an eye on her underlings so that they wouldn't be tempted to chat away the whole working day. The air conditioner had broken making the office hellishly hot. The manager had placed an order for a large fan so that it would be cooler. She'd made sure that it would be placed somewhere to the left of the watercooler so that she could keep an eye on it and control the settings if she needed to.</v>
       </c>
       <c r="G13">
         <v>13</v>
@@ -3749,38 +3816,38 @@
         <v>11</v>
       </c>
       <c r="Z13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">The new fan has been delivered, where would the manager want it to be placed? </v>
       </c>
       <c r="AA13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>Leftward of the managers desk</v>
       </c>
       <c r="AB13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>Rightward of the managers desk</v>
       </c>
       <c r="AC13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>There is not enough information</v>
       </c>
       <c r="AD13">
         <v>1</v>
       </c>
       <c r="AE13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">The Barbeque is about to start, which office workers is the worst cook? </v>
       </c>
       <c r="AF13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">Ella </v>
       </c>
       <c r="AG13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Felix</v>
       </c>
       <c r="AH13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>There is not enough information</v>
       </c>
       <c r="AI13">
@@ -3791,17 +3858,21 @@
       <c r="B14">
         <v>14</v>
       </c>
-      <c r="C14" t="s">
-        <v>314</v>
-      </c>
-      <c r="D14" t="s">
-        <v>400</v>
-      </c>
-      <c r="E14" t="s">
-        <v>401</v>
-      </c>
-      <c r="F14" t="s">
-        <v>402</v>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>Three difficult custom jobs had come to Daren's workshop in one day. This was most unusual, most of the time he struggled to get 3 jobs in one week, let alone in a day. He was going to need some help. Daren was a much better metal worker than his friend Steve but he needed his help none the less. They were friends and the work was sure to go smoothly. Toby was relatively new to the trade but was a good worker none the less, he obviously wasn't as good as Daren but he would still be a valuable asset while working on the 3 jobs.</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Three difficult custom jobs had come to Daren's workshop in one day. This was most unusual, most of the time he struggled to get 3 jobs in one week, let alone in a day. He was going to need some help. Daren was a much better metal worker than his friend Steve but he needed his help none the less. They were friends and the work was sure to go smoothly. Toby was relatively new to the trade but was a good worker none the less, he was obviously better than Daren and he would be a valuable asset while working on the 3 jobs. </v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">The metal workshop on Yew street had been there since the 1500s and as a result had expanded over the many years of operation. In front of a modern lathe stood a desk with a chair that was used as a mini office. This place was more about metal work than paper work but paper work had to be done nonetheless. Workers had recently noticed some small corners of paper had been chewed off which made them suspect that there was a mouse living somewhere behind the desk. It couldn't be in front of the desk simply because that concrete had only recently been repaired. </v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">The metal workshop on Yew street had been there since the 1500s and as a result had expanded over the many years of operation. In front of a modern lathe stood a desk with a chair that was used as a mini office. This place was more about metal work than paper work but paper work had to be done nonetheless. Workers had recently noticed some small corners of paper had been chewed off which made them suspect that there was a mouse living somewhere in front of the desk. It couldn't be behind of the desk simply because that concrete had only recently been repaired. </v>
       </c>
       <c r="G14">
         <v>14</v>
@@ -3861,38 +3932,38 @@
         <v>11</v>
       </c>
       <c r="Z14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>Daren has decided to set up a humane trap for the mouse where should he put it?</v>
       </c>
       <c r="AA14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">Behind the lathe </v>
       </c>
       <c r="AB14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>In front of the lathe</v>
       </c>
       <c r="AC14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>There is not enough information</v>
       </c>
       <c r="AD14">
         <v>2</v>
       </c>
       <c r="AE14" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>The least skilled worker in the workshop was always made to clean at the end of the day, who is this likely to be?</v>
       </c>
       <c r="AF14" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">Toby </v>
       </c>
       <c r="AG14" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">Steve </v>
       </c>
       <c r="AH14" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>There is not enough information</v>
       </c>
       <c r="AI14">
@@ -3903,17 +3974,21 @@
       <c r="B15">
         <v>15</v>
       </c>
-      <c r="C15" t="s">
-        <v>403</v>
-      </c>
-      <c r="D15" t="s">
-        <v>135</v>
-      </c>
-      <c r="E15" t="s">
-        <v>404</v>
-      </c>
-      <c r="F15" t="s">
-        <v>405</v>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">The workers of the copper mine were celebrating their recent pay rises at the local pub. All of them had been awarded a bonus based on their work experience at the mine and their productivity. Darius was happy, while it was true that he hadn't received as big of bonus as Belinda, he was still happy that he would be able to pay off a large proportion of his mortgage. Lucy was also happy with her bonus, she had received more than Darius and was already planning the extravagant holiday she would go on. </v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="1"/>
+        <v>The workers of the copper mine were celebrating their recent pay rises at the local pub. All of them had been awarded a bonus based on their work experience at the mine and their productivity. Darius was happy, while it was true that he hadn't received as big of bonus as Belinda, he was still happy that he would be able to pay off a large proportion of his mortgage. Lucy was also happy with her bonus, she hadn't received more than Darius but was already planning the extravagant holiday she would go on.</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">The mine had been a source of copper for almost 50 years. It wasn't particularly big, the company that owned it was small and couldn't afford to expand. Instead they enjoyed a steady stream of revenue and a constant influx of highly skilled workers. Shaft-A was currently the most profitable shaft and was situated somewhere below Shaft-B which had run dry a few years ago and was now used as a storage area. A recent exploratory drilling somewhere above Shaft-A and had revealed a good deposit of a very copper rich ore. </v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">The mine had been a source of copper for almost 50 years. It wasn't particularly big, the company that owned it was small and couldn't afford to expand. Instead they enjoyed a steady stream of revenue and a constant influx of highly skilled workers. Shaft-A was currently the most profitable shaft and was situated somewhere below Shaft-B which had run dry a few years ago and was now used as a storage area. A recent exploratory drilling somewhere below Shaft-A and had revealed a good deposit of a very copper rich ore. </v>
       </c>
       <c r="G15">
         <v>15</v>
@@ -3973,38 +4048,38 @@
         <v>11</v>
       </c>
       <c r="Z15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>The foreman is in the storage area, which way does he need to go to take a look at the newly discovered rich deposit of ore?</v>
       </c>
       <c r="AA15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>Up</v>
       </c>
       <c r="AB15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">Down </v>
       </c>
       <c r="AC15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>There is not enough information</v>
       </c>
       <c r="AD15">
         <v>2</v>
       </c>
       <c r="AE15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">A tax investigation is launched that will assess work place bonuses. Who has received the biggest bonus out of Lucy and Linda? </v>
       </c>
       <c r="AF15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Lucy</v>
       </c>
       <c r="AG15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">Belinda </v>
       </c>
       <c r="AH15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>There is not enough information</v>
       </c>
       <c r="AI15">
@@ -4015,17 +4090,21 @@
       <c r="B16">
         <v>16</v>
       </c>
-      <c r="C16" t="s">
-        <v>406</v>
-      </c>
-      <c r="D16" t="s">
-        <v>407</v>
-      </c>
-      <c r="E16" t="s">
-        <v>146</v>
-      </c>
-      <c r="F16" t="s">
-        <v>147</v>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Jolene was busy serving up noodles from her noodle van in the spot that she had had since the food festival began several years ago. She used to be the only one that sold noodles at the festival but this year she had two competitors. Jolene's noodles weren't as expensive as Tommy's noodles which meant that she was still getting a fair amount of business. Her other competitor, Fanella, also was not as expensive as Tommy. Jolene didn't actually mind all that much, the festival was big enough for the three of them. </v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Jolene was busy serving up noodles from her noodle van in the spot that she had had since the food festival began several years ago. She used to be the only one that sold noodles at the festival but this year she had two competitors. Jolene's noodles weren't as expensive as Tommy's noodles which meant that she was still getting a fair amount of business. Her other competitor, Fanella, had noodles that were more expensive than Tommy's. Jolene didn't actually mind all that much, the festival was big enough for the three of them. </v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="6"/>
+        <v>The food and wine festival was held every year in the Swampscott town square. It was growing year on year. To the left of the entrance were several posters for the upcoming events that made the festival special. Along with the usual fare of eating competitions there were sack races, dog shows and live music. Much to the dismay of many attendees, the wine drinking competition would not be held this year. Somewhere to the left of the entrance was a tent that was used as the festival's lost and found zone.</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="7"/>
+        <v>The food and wine festival was held every year in the Swampscott town square. It was growing year on year. To the left of the entrance were several posters for the upcoming events that made the festival special. Along with the usual fare of eating competitions there were sack races, dog shows and live music. Much to the dismay of many attendees, the wine drinking competition would not be held this year. Somewhere to the right of the entrance was a tent that was used as the festival's lost and found zone.</v>
       </c>
       <c r="G16">
         <v>16</v>
@@ -4064,7 +4143,7 @@
         <v>3</v>
       </c>
       <c r="S16" t="s">
-        <v>152</v>
+        <v>649</v>
       </c>
       <c r="T16" t="s">
         <v>153</v>
@@ -4085,38 +4164,38 @@
         <v>11</v>
       </c>
       <c r="Z16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">Tommy has lost his backpack, he is standing in front of the posters facing them, which way does he need to go to get to the lost and found tent? </v>
       </c>
       <c r="AA16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>Left</v>
       </c>
       <c r="AB16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>Right</v>
       </c>
       <c r="AC16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>There is not enough information</v>
       </c>
       <c r="AD16">
         <v>2</v>
       </c>
       <c r="AE16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Young festival goers tend to go for the cheapest noodles. Who's noodles are they most likely to eat?</v>
       </c>
       <c r="AF16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Jolene's</v>
       </c>
       <c r="AG16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Fanella's</v>
       </c>
       <c r="AH16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>There is not enough information</v>
       </c>
       <c r="AI16">
@@ -4127,17 +4206,21 @@
       <c r="B17">
         <v>17</v>
       </c>
-      <c r="C17" t="s">
-        <v>408</v>
-      </c>
-      <c r="D17" t="s">
-        <v>409</v>
-      </c>
-      <c r="E17" t="s">
-        <v>410</v>
-      </c>
-      <c r="F17" t="s">
-        <v>411</v>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">The town of Rockport boasted three major events that always drew in large amounts of crowds. There were also a few smaller events for locals in the summer. The Folk music festival drew in a much larger crowd than the Rockport Grand Prix. Both were important sources of income in the town. The Sailing festival was also more popular the Rockport Grand Prix but this didn't matter to the townsfolk. Rockport was one of the most up and coming towns in the area. The yearly events were beginning to draw in crowds from further and further afield. </v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">The town of Rockport boasted three major events that always drew in large amounts of crowds. There were also a few smaller events for locals in the summer. The Folk music festival drew in a much larger crowd than the Rockport Grand Prix. Both were important sources of income in the town. The Sailing festival was less popular the Rockport Grand Prix but this didn't matter to the townsfolk. Rockport was one of the most up and coming towns in the area. The yearly events were beginning to draw in crowds from further and further afield. </v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">The Rockport Grand Prix was anything but grand. It was a go-cart race for the under 15s and none of the carts could go about 30 miles per hour. The Blue team was one of the best in Rockport and was currently in front of the Red team. The coaches were happy about this as they had to beat the Red and Green team to qualify for the finals. The Green team were also ahead of the Reds. The Grand Prix was always a popular event in Rockport and would draw in onlookers from miles around. </v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">The Rockport Grand Prix was anything but grand. It was a go-cart race for the under 15s and none of the carts could go about 30 miles per hour. The Blue team was one of the best in Rockport and was currently in front of the Red team. The coaches were happy about this as they had to beat the Red and Green team to qualify for the finals. The Green team were behind of the Reds. The Grand Prix was always a popular event in Rockport and would draw in onlookers from miles around. </v>
       </c>
       <c r="G17">
         <v>17</v>
@@ -4197,38 +4280,38 @@
         <v>11</v>
       </c>
       <c r="Z17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>Based on current position, which team is most likely to win?</v>
       </c>
       <c r="AA17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>The blue team</v>
       </c>
       <c r="AB17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>The green team</v>
       </c>
       <c r="AC17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>There is not enough information</v>
       </c>
       <c r="AD17">
         <v>1</v>
       </c>
       <c r="AE17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Based on their popularity, which festival is likely to have the most attendees?</v>
       </c>
       <c r="AF17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">The folk music festival </v>
       </c>
       <c r="AG17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">The sailing festival </v>
       </c>
       <c r="AH17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>There is not enough information</v>
       </c>
       <c r="AI17">
@@ -4239,17 +4322,21 @@
       <c r="B18">
         <v>18</v>
       </c>
-      <c r="C18" t="s">
-        <v>412</v>
-      </c>
-      <c r="D18" t="s">
-        <v>413</v>
-      </c>
-      <c r="E18" t="s">
-        <v>323</v>
-      </c>
-      <c r="F18" t="s">
-        <v>322</v>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>The Kingsley hills tourism board were looking to build a museum to display the archaeological findings of the area. The board were looking for local businesses to co-fund the project. Farmer Jack's farm shop was eager to fund the project. However, Farmer Jack's were not as wealthy as The Pepper Mills Hotel. So couldn't offer as much money as them.The local bus company also wanted to co-fund the project. They were not as wealthy as the Pepper Mills hotel. The tourism board were sure that they would have all they needed to build the museum.</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">The Kingsley hills tourism board were looking to build a museum to display the archaeological findings of the area. The board were looking for local businesses to co-fund the project. Farmer Jack's farm shop was eager to fund the project. However, Farmer Jack's were not as wealthy as The Pepper Mills Hotel. So couldn't offer as much money as them. The local bus company also wanted to co-fund the project. They were even wealthier than The Pepper Mills hotel. The tourism board were sure would have all they needed to build the museum. </v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="6"/>
+        <v>The Kingsley hills were an area of great archaeological importance. There was a small rest stop somewhere below a small fully excavated dig site. The site had yielded many interesting finds that shed light on the daily lives of early Anglo-Saxon settlers in England. Somewhere downhill of this site was a small patch of grass that never grew quite as tall as the grass around it. This was evidence of another point of interest and a potential dig site. The archaeological work in the hills was often suspended in the summer due to the influx of tourists.</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="7"/>
+        <v>The Kingsley hills were an area of great archaeological importance. There was a small rest stop somewhere below a small fully excavated dig site. The site had yielded many interesting finds that shed light on the daily lives of early Anglo-Saxon settlers in England. Somewhere uphill of this site was a small patch of grass that never grew quite as tall as the grass around it. This was evidence of another point of interest and a potential dig site. The archaeological work in the hills was often suspended in the summer due to the influx of tourists.</v>
       </c>
       <c r="G18">
         <v>18</v>
@@ -4288,7 +4375,7 @@
         <v>3</v>
       </c>
       <c r="S18" t="s">
-        <v>172</v>
+        <v>648</v>
       </c>
       <c r="T18" t="s">
         <v>173</v>
@@ -4309,38 +4396,38 @@
         <v>11</v>
       </c>
       <c r="Z18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>An archaeologist has gone to the potential dig site and wants to get to the rest stop. Which way does he need to go?</v>
       </c>
       <c r="AA18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>Up the hill</v>
       </c>
       <c r="AB18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">Down the hill </v>
       </c>
       <c r="AC18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>There is not enough information</v>
       </c>
       <c r="AD18">
         <v>2</v>
       </c>
       <c r="AE18" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Which local company is likely to put the least amount of money toward tourism board's project?</v>
       </c>
       <c r="AF18" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Farmer Jack's farm</v>
       </c>
       <c r="AG18" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">The bus company </v>
       </c>
       <c r="AH18" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>There is not enough information</v>
       </c>
       <c r="AI18">
@@ -4351,17 +4438,21 @@
       <c r="B19">
         <v>19</v>
       </c>
-      <c r="C19" t="s">
-        <v>414</v>
-      </c>
-      <c r="D19" t="s">
-        <v>415</v>
-      </c>
-      <c r="E19" t="s">
-        <v>325</v>
-      </c>
-      <c r="F19" t="s">
-        <v>416</v>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Alfred McMurphy had managed the pub ever since his father had retired several years ago. It was a family operation and always had been. Frank McMurphy wasn't as popular with the patrons as his brother Alfred but they liked him well enough. They were all popular when they served the drinks and listened to patrons' woes. Susan McMurphy also worked at the pub and was also not as popular as her brother Alfred. It didn't matter of course, to the McMurphy's Family always came first. </v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Alfred McMurphy had managed the pub ever since his father had retired several years ago. It was a family operation and always had been. Frank McMurphy wasn't as popular with the patrons as his brother Alfred but they liked him well enough. They were all popular when they served the drinks and listened to patrons' woes. Susan McMurphy also worked at the pub and was a lot more popular as her brother Alfred. It didn't matter of course, to the McMurphy's Family always came first. </v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="6"/>
+        <v>McMurphy's Pub was one of the best in Amherst. The owners had decided to add additional seating so that they could serve more customers than ever before. To the right of the central row of tables was the bar, which was almost as long as the whole pub itself. There were barstools along the whole bar and were considered to be the best seats in the house. To the left of the bar was an old jukebox that played records from the 70s and 80s. On a Friday night the place was absolutely full, especially if it was one of the bi-weekly live music nights.</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="7"/>
+        <v>McMurphy's Pub was one of the best in Amherst. The owners had decided to add additional seating so that they could serve more customers than ever before. To the right of the central row of tables was the bar, which was almost as long as the whole pub itself. There were barstools along the whole bar and were considered to be the best seats in the house. To the Right of the bar was an old jukebox that played records from the 70s and 80s. On a Friday night the place was absolutely full, especially if it was one of the bi-weekly live music nights.</v>
       </c>
       <c r="G19">
         <v>19</v>
@@ -4421,38 +4512,38 @@
         <v>11</v>
       </c>
       <c r="Z19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>Susan has just put her favourite song on the jukebox, she now wants to have a beer. Which way does she need to go to reach the bar?</v>
       </c>
       <c r="AA19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>Left</v>
       </c>
       <c r="AB19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>Right</v>
       </c>
       <c r="AC19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>There is not enough information</v>
       </c>
       <c r="AD19">
         <v>1</v>
       </c>
       <c r="AE19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">All of the McMurphy's are well liked by their patrons but who is the least popular among the three of them? </v>
       </c>
       <c r="AF19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Frank</v>
       </c>
       <c r="AG19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Susan</v>
       </c>
       <c r="AH19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>There is not enough information</v>
       </c>
       <c r="AI19">
@@ -4463,17 +4554,21 @@
       <c r="B20">
         <v>20</v>
       </c>
-      <c r="C20" t="s">
-        <v>417</v>
-      </c>
-      <c r="D20" t="s">
-        <v>418</v>
-      </c>
-      <c r="E20" t="s">
-        <v>419</v>
-      </c>
-      <c r="F20" t="s">
-        <v>420</v>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">The Fishermen of Rockport would often gather in the Pub by the docks and relax after a day out at sea. Today though they'd all stayed on dry land as the regatta was taking place and no one wanted to get in the way. Todd was a skilled captain and loved to buy a round of drinks for the whole pub. Although he wasn't as good as Herman. Herman's son Melvin had recently purchased his own fishing boat and would head out with his own crew, though only a boy of 18 he was already a better fisherman than Todd. </v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">The Fishermen of Rockport would often gather in the Pub by the docks and relax after a day out at sea. Today though they'd all stayed on dry land as the regatta was taking place and no one wanted to get in the way. Todd was a skilled captain and loved to buy a round of drinks for the whole pub. Although he wasn't as good as Herman. Herman's son Melvin had recently purchased his own fishing boat and would head out with his own crew, though only a boy of 18 he still wasn't a better fisherman than Todd. </v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">The annual sailing festival had started as it always did with the sailing regatta. Three teams from Rockport had entered the regatta in the hope of winning. The crew of the Royal Lady had managed to get a good start but were behind the King Fisher's crew. The weather was perfect for sailing that day and made for much better conditions than the previous years. The third crew from Rockport on the boat the Fast Kitten were also ahead of the Royal Lady. This was going to be an exciting race and the locals cheered on the crews from Rockport as they sailed past them. </v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">The annual sailing festival had started as it always did with the sailing regatta. Three teams from Rockport had entered the regatta in the hope of winning. The crew of the Royal Lady had managed to get a good start but were behind the King Fisher's crew. The weather was perfect for sailing that day and made for much better conditions than the previous years. The third crew from Rockport on the boat the Fast Kitten were behind of the Royal Lady. This was going to be an exciting race and the locals cheered on the crews from Rockport as they sailed past them. </v>
       </c>
       <c r="G20">
         <v>20</v>
@@ -4533,38 +4628,38 @@
         <v>11</v>
       </c>
       <c r="Z20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>Which sailing boat from Rockport is currently ahead of the others?</v>
       </c>
       <c r="AA20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>The King Fisher</v>
       </c>
       <c r="AB20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>The Fast Kitten</v>
       </c>
       <c r="AC20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>There is not enough information</v>
       </c>
       <c r="AD20">
         <v>1</v>
       </c>
       <c r="AE20" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Who is the most skilled fisherman currently in the Rockport pub?</v>
       </c>
       <c r="AF20" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Melvin</v>
       </c>
       <c r="AG20" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Herman</v>
       </c>
       <c r="AH20" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>There is not enough information</v>
       </c>
       <c r="AI20">
@@ -4575,17 +4670,21 @@
       <c r="B21">
         <v>21</v>
       </c>
-      <c r="C21" t="s">
-        <v>421</v>
-      </c>
-      <c r="D21" t="s">
-        <v>422</v>
-      </c>
-      <c r="E21" t="s">
-        <v>327</v>
-      </c>
-      <c r="F21" t="s">
-        <v>326</v>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">There are a few teams hoping to find Archaeological evidence of Dogger bank settlements that operate in the north sea. The Norwegians have much more funding than the British. Their equipment is proof of this as it's some of the most modern equipment on the market. This didn't mean that anyone was actively working against each other though. As in all sciences, working together is key. The Danish team's also have less funding than the Norwegians but they still share their findings with everyone just as the British do. </v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">There are a few teams hoping to find Archaeological evidence of Dogger bank settlements that operate in the north sea. The Norwegians have much more funding than the British. Their equipment is proof of this as it's some of the most modern equipment on the market. This didn't mean that anyone was actively working against each other though. As in all sciences, working together is key. The Danish team's funding was better than the Norwegians but they still share their findings with everyone just as the British do. </v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="6"/>
+        <v>Dogger Bank in the North Sea is thought to be one of the most significant locations for evidence of early Neolithic settlements. There is only one problem, it is under water. A team of divers and archaeologists were performing a study of the area. They had sent in two submarines and a small team of divers. The submarine in charge of taking pictures was somewhere above the divers who were adjusting to the pressure before they dove lower. Somewhere below the submarine taking pictures was the second submarine, which would be used to transport anything the divers found.</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="7"/>
+        <v>Dogger Bank in the North Sea is thought to be one of the most significant locations for evidence of early Neolithic settlements. There is only one problem, it is under water. A team of divers and archaeologists were performing a study of the area. They had sent in two submarines and a small team of divers. The submarine in charge of taking pictures was somewhere above the divers who were adjusting to the pressure before they dove lower. Somewhere above the submarine taking pictures was the second submarine, which would be used to transport anything the divers found.</v>
       </c>
       <c r="G21">
         <v>21</v>
@@ -4645,38 +4744,38 @@
         <v>11</v>
       </c>
       <c r="Z21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">The submarine used to transport finds has malfunctioned, which way do the divers need to swim in order to fix it? </v>
       </c>
       <c r="AA21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>Up</v>
       </c>
       <c r="AB21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>Down</v>
       </c>
       <c r="AC21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>There is not enough information</v>
       </c>
       <c r="AD21">
         <v>1</v>
       </c>
       <c r="AE21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">The least well funded team is going to be responsible for washing any artifacts found, which team is this likely to be? </v>
       </c>
       <c r="AF21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Great Britian's</v>
       </c>
       <c r="AG21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Denmark's</v>
       </c>
       <c r="AH21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>There is not enough information</v>
       </c>
       <c r="AI21">
@@ -4687,17 +4786,21 @@
       <c r="B22">
         <v>22</v>
       </c>
-      <c r="C22" t="s">
-        <v>423</v>
-      </c>
-      <c r="D22" t="s">
-        <v>424</v>
-      </c>
-      <c r="E22" t="s">
-        <v>425</v>
-      </c>
-      <c r="F22" t="s">
-        <v>426</v>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">The catering company hired to provide food for the big pool party was having problems. Many of their usual staff had called in sick. This meant that the company were now desperately scrambling to get their best staff to come in. Amanda wasn't as skilled as Sammy who was always eager to help out. Besides, Sammy always needed the money. There was of course the option of asking Jess to come in. Jess wasn't as skilled as Sammy. The catering company boss hoped everything would run smoothly. </v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">The catering company hired to provide food for the big pool party was having problems. Many of their usual staff had called in sick. This meant that the company were now desperately scrambling to get their best staff to come in. Amanda wasn't as skilled as Sammy who was always eager to help out. Besides, Sammy always needed the money. There was of course the option of asking Jess to come in. Jess was more skilled than Sammy. The catering company boss hoped everything would run smoothly. </v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">The community pool was having its annual party. To the right of the pool's ladder was the water filter which had been inspected and cleaned before the event. Staff wanted to be sure that everything was up to scratch. The pool was in a better condition than ever this year due to refurbishments that had finished just before summer, the whole staff were very pleased with the results. Though one thing that was overlooked was a small paving slab that had come loose somewhere to the right of the pool's ladder. Hopefully no one would trip over it. </v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">The community pool was having its annual party. To the right of the pool's ladder was the water filter which had been inspected and cleaned before the event. Staff wanted to be sure that everything was up to scratch. The pool was in a better condition than ever this year due to refurbishments that had finished just before summer, the whole staff were very pleased with the results. Though one thing that was overlooked was a small paving slab that had come loose somewhere to the left of the pool's ladder. Hopefully no one would trip over it. </v>
       </c>
       <c r="G22">
         <v>22</v>
@@ -4757,38 +4860,38 @@
         <v>11</v>
       </c>
       <c r="Z22" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">A lifeguard is standing in front of the water filter facing the pool. In which direction does he need to look to find the loose paving slab? </v>
       </c>
       <c r="AA22" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>Left</v>
       </c>
       <c r="AB22" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">Right </v>
       </c>
       <c r="AC22" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>There is not enough information</v>
       </c>
       <c r="AD22">
         <v>1</v>
       </c>
       <c r="AE22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>If the catering company wants only the most skilled workers for the pool party who is least likely to be asked to help?</v>
       </c>
       <c r="AF22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">Amanda </v>
       </c>
       <c r="AG22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Jess</v>
       </c>
       <c r="AH22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>There is not enough information</v>
       </c>
       <c r="AI22">
@@ -4799,17 +4902,21 @@
       <c r="B23">
         <v>23</v>
       </c>
-      <c r="C23" t="s">
-        <v>427</v>
-      </c>
-      <c r="D23" t="s">
-        <v>428</v>
-      </c>
-      <c r="E23" t="s">
-        <v>429</v>
-      </c>
-      <c r="F23" t="s">
-        <v>430</v>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Three business owners from Innsmouth were looking to support the local communities growing art community. They were planning to invest in the gallery. Fred who owned a small Café by the beach was hoping to get his hands on some driftwood pieces that he could display at his café. He wasn't going to be able to pledge as much Money as Geraldine who was trying to be elected as Mayor. Simon was also looking to pledge a decent amount of money to the gallery but was also not really able to match the amount that Geraldine was planning on giving. </v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Three business owners from Innsmouth were looking to support the local communities growing art community. They were planning to invest in the gallery. Fred who owned a small Café by the beach was hoping to get his hands on some driftwood pieces that he could display at his café. He wasn't going to be able to pledge as much Money as Geraldine who was trying to be elected as Mayor. Simon was also looking to pledge a decent amount of money to the gallery was also able to double the amount that Geraldine was planning on giving. </v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">The art gallery of Innsmouth was holding an exhibition for local artists. Innsmouth was small and word had gotten around quickly. The Local artist's work was on display throughout a large hall with visitors walking past paintings and sculptures. A sculpture made of driftwood stood behind a smaller sculpture of a Whale at the centre of the hall. Somewhere behind the sculpture of a Whale stood a horrible piece made from washed up plastic bottles, which was not very popular among the locals. Overall the exhibition was looking to be a grand success. </v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">The art gallery of Innsmouth was holding an exhibition for local artists. Innsmouth was small and word had gotten around quickly. The Local artist's work was on display throughout a large hall with visitors walking past paintings and sculptures. A sculpture made of driftwood stood behind a smaller sculpture of a Whale at the centre of the hall. Somewhere in front of the sculpture of a Whale stood a horrible piece made from washed up plastic bottles, which was not very popular among the locals. Overall the exhibition was looking to be a grand success. </v>
       </c>
       <c r="G23">
         <v>23</v>
@@ -4869,38 +4976,38 @@
         <v>11</v>
       </c>
       <c r="Z23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>Fred is standing by the Sculpture made of driftwood, in which general direction does he need to go to get to the sculpture made of plastic bottles?</v>
       </c>
       <c r="AA23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">Towards the sculpture of the whale </v>
       </c>
       <c r="AB23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">Away from the sculpture of the whale </v>
       </c>
       <c r="AC23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>There is not enough information</v>
       </c>
       <c r="AD23">
         <v>1</v>
       </c>
       <c r="AE23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Which of the three business owners is going to donate the least amount of money to the gallery?</v>
       </c>
       <c r="AF23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Fred</v>
       </c>
       <c r="AG23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">Simon </v>
       </c>
       <c r="AH23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>There is not enough information</v>
       </c>
       <c r="AI23">
@@ -4911,17 +5018,21 @@
       <c r="B24">
         <v>24</v>
       </c>
-      <c r="C24" t="s">
-        <v>221</v>
-      </c>
-      <c r="D24" t="s">
-        <v>431</v>
-      </c>
-      <c r="E24" t="s">
-        <v>432</v>
-      </c>
-      <c r="F24" t="s">
-        <v>433</v>
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>It had been some time since Josephine's and Aaron's family had come together, but this was their wedding so no one was going to miss out on it. The two had been together for years and both came from families where people considered themselves the heart and soul of the party. Aaron's father Gary was a great storyteller, much more so than Aaron was. Josephine also loved to spin yarns but wasn't as good as Gary. The wedding reception and ceremony was bound to be a battleground of sorts as to who would tell the best story.</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">It had been some time since Josephine's and Aarron's family had come together, but this was their wedding so no one was going to miss out on it. The two had been together for years and both came from families where people considered themselves the heart and soul of the party. Aarron's father Gary was a great storyteller, much more so than Aaron was. Josephine also loved to spin yarns and was better than Gary. The wedding reception and ceremony was bound to be a battleground of sorts as to who would tell the best story. </v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">The cemetery was old and within it many trees grew. They had almost outgrown the spire of the chapel they surrounded. The Oaks towered above the yew trees. The trees that grew in the cemetery gave plenty of shade so it was never too hot for those that visited their passed relatives in the summer. The Birch trees also towered above the Yews and when they shed their paper like bark it was often confused with confetti left over from a wedding at the chapel. This was a popular spot for weddings, as the trees and the old stonework provided a beautiful backdrop for photos. </v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">The cemetery was old and within it many trees grew. They had almost outgrown the spire of the chapel they surrounded. The Oaks towered above the yew trees. The trees that grew in the cemetery gave plenty of shade so it was never too hot for those that visited their passed relatives in the summer. The Birch trees were not as tall as the Yews but when they shed their paper like bark it was often confused with confetti left over from a wedding at the chapel. This was a popular spot for weddings, as the trees and the old stonework provided a beautiful backdrop for photos. </v>
       </c>
       <c r="G24">
         <v>24</v>
@@ -4981,38 +5092,38 @@
         <v>11</v>
       </c>
       <c r="Z24" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>A recent storm has brought down the tallest tree in the cemetary, which type of tree is most likely to have fallen?</v>
       </c>
       <c r="AA24" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>Oak</v>
       </c>
       <c r="AB24" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>Birch</v>
       </c>
       <c r="AC24" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>There is not enough information</v>
       </c>
       <c r="AD24">
         <v>1</v>
       </c>
       <c r="AE24" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">The wedding will have many speeches and anecdotes but who is likely to tell the best story? </v>
       </c>
       <c r="AF24" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Aaron</v>
       </c>
       <c r="AG24" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Josephine</v>
       </c>
       <c r="AH24" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>There is not enough information</v>
       </c>
       <c r="AI24">
@@ -5023,17 +5134,21 @@
       <c r="B25">
         <v>25</v>
       </c>
-      <c r="C25" t="s">
-        <v>234</v>
-      </c>
-      <c r="D25" t="s">
-        <v>235</v>
-      </c>
-      <c r="E25" t="s">
-        <v>434</v>
-      </c>
-      <c r="F25" t="s">
-        <v>435</v>
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>Naomi had always been curious about the many abandoned pieces of equipment that littered the fields around her home. She was very brave for her age but wasn't as brave as her little sister Jane. Jane could find adventure where ever she went. Sometimes, when their older brother Will came home from school, the three would go off exploring the countryside together. Will wasn't as brave as Jane but they loved to pretend that they were explorers in some vast unknown land.</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="1"/>
+        <v>Naomi had always been curious about the many abandoned pieces of equipment that littered the fields around her home. She was very brave for her age but wasn't as brave as her little sister Jane. Jane could find adventure where ever she went. Sometimes, when their older brother Will came home from school, the three would go off exploring the countryside together. Will was braver than Jane and they loved to pretend that they were explorers in some vast unknown land.</v>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">The farm that lay on the outskirts of town was large but had fallen into disrepair To the left of the only barn still in use stood a rusty old tractor. Most of the equipment had accumulated so much rust that all of it looked a reddish brown regardless of what colour it had been before. The only regularly used piece of equipment was a quad bike which stood somewhere to the left of the barn. If the quad bike was to break it would spell disaster for the farmer and his family who were holding on to their property by a string. </v>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">The farm that lay on the outskirts of town was large but had fallen into disrepair. To the left of the only barn still in use stood a rusty old tractor. Most of the equipment had accumulated so much rust that all of it looked a reddish brown regardless of what colour it had been before. The only regularly used piece of equipment was a quad bike which stood somewhere to the right of the barn. If the quad bike was to break it would spell disaster for the farmer and his family who were holding on to their property by a string. </v>
       </c>
       <c r="G25">
         <v>25</v>
@@ -5087,38 +5202,38 @@
         <v>2</v>
       </c>
       <c r="Z25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">The Farmer is standing by the rusty tractor facing it, which way does he need to go to get to his quad bike? </v>
       </c>
       <c r="AA25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>Right</v>
       </c>
       <c r="AB25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">Left </v>
       </c>
       <c r="AC25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">There is not enough information </v>
       </c>
       <c r="AD25">
         <v>1</v>
       </c>
       <c r="AE25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>All of the siblings are braver than average but which of them is the bravest?</v>
       </c>
       <c r="AF25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Will</v>
       </c>
       <c r="AG25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Jane</v>
       </c>
       <c r="AH25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>There is not enough information</v>
       </c>
       <c r="AI25">
@@ -5129,17 +5244,21 @@
       <c r="B26">
         <v>26</v>
       </c>
-      <c r="C26" t="s">
-        <v>244</v>
-      </c>
-      <c r="D26" t="s">
-        <v>244</v>
-      </c>
-      <c r="E26" t="s">
-        <v>245</v>
-      </c>
-      <c r="F26" t="s">
-        <v>245</v>
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>The three women had long wanted to put the sailing skills they'd learned in their youth to good use. Holly was a much better sailor than Vicky, because Holly had learned to sail from her father at a young age. Julie on the other hand wasn't as good at sailing as Vicky as she had only moved to Plum Island in her teenage years. Despite the differences in their abilities, the three loved to race one another and truly test themselves against the strong winds of the Atlantic.</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="1"/>
+        <v>The three women had long wanted to put the sailing skills they'd learned in their youth to good use. Holly was a much better sailor than Vicky, because Holly had learned to sail from her father at a young age. Julie on the other hand wasn't as good at sailing as Vicky as she had only moved to Plum Island in her teenage years. Despite the differences in their abilities, the three loved to race one another and truly test themselves against the strong winds of the Atlantic.</v>
+      </c>
+      <c r="E26" t="str">
+        <f t="shared" si="6"/>
+        <v>The passenger ferry to Plum Island had broken down, that much was clear. What was not clear was which boat would replace it. A new, bright red boat was docked to the right of the broken down ferry. Because it was new, the red boat would be more expensive to rent but the ferry company would have to make a choice. To the left of the broken down ferry was an older, rusty brown tug boat. It wasn't as new but could transport more people at one time. The ferry company would have to make a choice sooner rather than later.</v>
+      </c>
+      <c r="F26" t="str">
+        <f t="shared" si="7"/>
+        <v>The passenger ferry to Plum Island had broken down, that much was clear. What was not clear was which boat would replace it. A new, bright red boat was docked to the right of the broken down ferry. Because it was new, the red boat would be more expensive to rent but the ferry company would have to make a choice. To the left of the broken down ferry was an older, rusty brown tug boat. It wasn't as new but could transport more people at one time. The ferry company would have to make a choice sooner rather than later.</v>
       </c>
       <c r="G26">
         <v>26</v>
@@ -5193,38 +5312,38 @@
         <v>2</v>
       </c>
       <c r="Z26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>Vicky is standing in front of the broken down ferry facing it, which way does she need to go in order to stand infront of the red boat?</v>
       </c>
       <c r="AA26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>Right</v>
       </c>
       <c r="AB26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">Left </v>
       </c>
       <c r="AC26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">There is not enough information </v>
       </c>
       <c r="AD26">
         <v>1</v>
       </c>
       <c r="AE26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">The three women are planning to have a race. Based on their sailing ability, which one is most likely to win? </v>
       </c>
       <c r="AF26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Holly</v>
       </c>
       <c r="AG26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Vicky</v>
       </c>
       <c r="AH26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>There is not enough information</v>
       </c>
       <c r="AI26">
@@ -5337,7 +5456,7 @@
     </row>
     <row r="31" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
-        <f t="shared" ref="A31:A56" si="2">IF(ABS(D31-F31)&lt;30,"GOOD","BAD")</f>
+        <f t="shared" ref="A31:A56" si="8">IF(ABS(D31-F31)&lt;30,"GOOD","BAD")</f>
         <v>GOOD</v>
       </c>
       <c r="B31">
@@ -5422,7 +5541,7 @@
     </row>
     <row r="32" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>GOOD</v>
       </c>
       <c r="B32">
@@ -5432,64 +5551,64 @@
         <v>12</v>
       </c>
       <c r="D32">
-        <f t="shared" ref="D32:D56" si="3">LEN(C32)</f>
+        <f t="shared" ref="D32:D56" si="9">LEN(C32)</f>
         <v>565</v>
       </c>
       <c r="E32" t="s">
         <v>13</v>
       </c>
       <c r="F32">
-        <f t="shared" ref="F32:F56" si="4">LEN(E32)</f>
+        <f t="shared" ref="F32:F56" si="10">LEN(E32)</f>
         <v>549</v>
       </c>
       <c r="G32" t="s">
         <v>287</v>
       </c>
       <c r="H32">
-        <f t="shared" ref="H32:H56" si="5">LEN(G32)</f>
+        <f t="shared" ref="H32:H56" si="11">LEN(G32)</f>
         <v>536</v>
       </c>
       <c r="I32" t="s">
         <v>286</v>
       </c>
       <c r="J32">
-        <f t="shared" ref="J32:J56" si="6">LEN(I32)</f>
+        <f t="shared" ref="J32:J56" si="12">LEN(I32)</f>
         <v>536</v>
       </c>
       <c r="L32">
-        <f t="shared" ref="L32:L56" si="7">SUM(D32,F32)/2</f>
+        <f t="shared" ref="L32:L56" si="13">SUM(D32,F32)/2</f>
         <v>557</v>
       </c>
       <c r="M32">
-        <f t="shared" ref="M32:M56" si="8">SUM(H32,J32)/2</f>
+        <f t="shared" ref="M32:M56" si="14">SUM(H32,J32)/2</f>
         <v>536</v>
       </c>
       <c r="N32">
-        <f t="shared" ref="N32:N56" si="9">SUM(L32:M32)</f>
+        <f t="shared" ref="N32:N56" si="15">SUM(L32:M32)</f>
         <v>1093</v>
       </c>
       <c r="O32" t="str">
-        <f t="shared" ref="O32:O56" si="10">IF(N32&lt;1100,"Good","Bad")</f>
+        <f t="shared" ref="O32:O56" si="16">IF(N32&lt;1100,"Good","Bad")</f>
         <v>Good</v>
       </c>
       <c r="P32" t="str">
-        <f t="shared" ref="P32:P56" si="11">IF(ABS(L32-M32)&gt;70,"BAD","GOOD")</f>
+        <f t="shared" ref="P32:P56" si="17">IF(ABS(L32-M32)&gt;70,"BAD","GOOD")</f>
         <v>GOOD</v>
       </c>
       <c r="Q32" t="str">
-        <f t="shared" ref="Q32:Q56" si="12">IF(ABS(H32-J32)&gt;50,"BAD","GOOD")</f>
+        <f t="shared" ref="Q32:Q56" si="18">IF(ABS(H32-J32)&gt;50,"BAD","GOOD")</f>
         <v>GOOD</v>
       </c>
       <c r="R32" t="str">
-        <f t="shared" ref="R32:R56" si="13">IF(ABS(D32-F32)&gt;50,"BAD","GOOD")</f>
+        <f t="shared" ref="R32:R56" si="19">IF(ABS(D32-F32)&gt;50,"BAD","GOOD")</f>
         <v>GOOD</v>
       </c>
       <c r="S32">
-        <f t="shared" ref="S32:S56" si="14">N32/75</f>
+        <f t="shared" ref="S32:S56" si="20">N32/75</f>
         <v>14.573333333333334</v>
       </c>
       <c r="T32" t="str">
-        <f t="shared" ref="T32:T56" si="15">IF(ABS(H32-J32)&lt;30,"GOOD","BAD")</f>
+        <f t="shared" ref="T32:T56" si="21">IF(ABS(H32-J32)&lt;30,"GOOD","BAD")</f>
         <v>GOOD</v>
       </c>
       <c r="U32">
@@ -5497,17 +5616,17 @@
         <v>8</v>
       </c>
       <c r="V32">
-        <f t="shared" ref="V32:V56" si="16">ROUNDUP(M32/75,0)</f>
+        <f t="shared" ref="V32:V56" si="22">ROUNDUP(M32/75,0)</f>
         <v>8</v>
       </c>
       <c r="W32">
-        <f t="shared" ref="W32:W56" si="17">U32+V32-1</f>
+        <f t="shared" ref="W32:W56" si="23">U32+V32-1</f>
         <v>15</v>
       </c>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>GOOD</v>
       </c>
       <c r="B33">
@@ -5517,82 +5636,82 @@
         <v>289</v>
       </c>
       <c r="D33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>500</v>
       </c>
       <c r="E33" t="s">
         <v>288</v>
       </c>
       <c r="F33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>500</v>
       </c>
       <c r="G33" t="s">
         <v>291</v>
       </c>
       <c r="H33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>527</v>
       </c>
       <c r="I33" t="s">
         <v>290</v>
       </c>
       <c r="J33">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>532</v>
       </c>
       <c r="L33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>500</v>
       </c>
       <c r="M33">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>529.5</v>
       </c>
       <c r="N33">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1029.5</v>
       </c>
       <c r="O33" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>Good</v>
       </c>
       <c r="P33" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>GOOD</v>
       </c>
       <c r="Q33" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>GOOD</v>
       </c>
       <c r="R33" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>GOOD</v>
       </c>
       <c r="S33">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>13.726666666666667</v>
       </c>
       <c r="T33" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>GOOD</v>
       </c>
       <c r="U33">
-        <f t="shared" ref="U33:U56" si="18">ROUNDUP(L33/75,0)</f>
+        <f t="shared" ref="U33:U56" si="24">ROUNDUP(L33/75,0)</f>
         <v>7</v>
       </c>
       <c r="V33">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>8</v>
       </c>
       <c r="W33">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>GOOD</v>
       </c>
       <c r="B34">
@@ -5602,82 +5721,82 @@
         <v>294</v>
       </c>
       <c r="D34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>525</v>
       </c>
       <c r="E34" t="s">
         <v>295</v>
       </c>
       <c r="F34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>519</v>
       </c>
       <c r="G34" t="s">
         <v>292</v>
       </c>
       <c r="H34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>549</v>
       </c>
       <c r="I34" t="s">
         <v>293</v>
       </c>
       <c r="J34">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>550</v>
       </c>
       <c r="L34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>522</v>
       </c>
       <c r="M34">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>549.5</v>
       </c>
       <c r="N34">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1071.5</v>
       </c>
       <c r="O34" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>Good</v>
       </c>
       <c r="P34" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>GOOD</v>
       </c>
       <c r="Q34" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>GOOD</v>
       </c>
       <c r="R34" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>GOOD</v>
       </c>
       <c r="S34">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>14.286666666666667</v>
       </c>
       <c r="T34" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>GOOD</v>
       </c>
       <c r="U34">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>7</v>
       </c>
       <c r="V34">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>8</v>
       </c>
       <c r="W34">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>GOOD</v>
       </c>
       <c r="B35">
@@ -5687,82 +5806,82 @@
         <v>299</v>
       </c>
       <c r="D35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>562</v>
       </c>
       <c r="E35" t="s">
         <v>298</v>
       </c>
       <c r="F35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>565</v>
       </c>
       <c r="G35" t="s">
         <v>296</v>
       </c>
       <c r="H35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>530</v>
       </c>
       <c r="I35" t="s">
         <v>297</v>
       </c>
       <c r="J35">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>530</v>
       </c>
       <c r="L35">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>563.5</v>
       </c>
       <c r="M35">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>530</v>
       </c>
       <c r="N35">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1093.5</v>
       </c>
       <c r="O35" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>Good</v>
       </c>
       <c r="P35" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>GOOD</v>
       </c>
       <c r="Q35" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>GOOD</v>
       </c>
       <c r="R35" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>GOOD</v>
       </c>
       <c r="S35">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>14.58</v>
       </c>
       <c r="T35" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>GOOD</v>
       </c>
       <c r="U35">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>8</v>
       </c>
       <c r="V35">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>8</v>
       </c>
       <c r="W35">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>15</v>
       </c>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>GOOD</v>
       </c>
       <c r="B36">
@@ -5772,82 +5891,82 @@
         <v>48</v>
       </c>
       <c r="D36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>446</v>
       </c>
       <c r="E36" t="s">
         <v>49</v>
       </c>
       <c r="F36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>437</v>
       </c>
       <c r="G36" t="s">
         <v>301</v>
       </c>
       <c r="H36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>500</v>
       </c>
       <c r="I36" t="s">
         <v>300</v>
       </c>
       <c r="J36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>497</v>
       </c>
       <c r="L36">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>441.5</v>
       </c>
       <c r="M36">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>498.5</v>
       </c>
       <c r="N36">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>940</v>
       </c>
       <c r="O36" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>Good</v>
       </c>
       <c r="P36" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>GOOD</v>
       </c>
       <c r="Q36" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>GOOD</v>
       </c>
       <c r="R36" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>GOOD</v>
       </c>
       <c r="S36">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>12.533333333333333</v>
       </c>
       <c r="T36" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>GOOD</v>
       </c>
       <c r="U36">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>6</v>
       </c>
       <c r="V36">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>7</v>
       </c>
       <c r="W36">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>12</v>
       </c>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>GOOD</v>
       </c>
       <c r="B37">
@@ -5857,82 +5976,82 @@
         <v>305</v>
       </c>
       <c r="D37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>517</v>
       </c>
       <c r="E37" t="s">
         <v>304</v>
       </c>
       <c r="F37">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>536</v>
       </c>
       <c r="G37" t="s">
         <v>302</v>
       </c>
       <c r="H37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>573</v>
       </c>
       <c r="I37" t="s">
         <v>303</v>
       </c>
       <c r="J37">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>564</v>
       </c>
       <c r="L37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>526.5</v>
       </c>
       <c r="M37">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>568.5</v>
       </c>
       <c r="N37">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1095</v>
       </c>
       <c r="O37" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>Good</v>
       </c>
       <c r="P37" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>GOOD</v>
       </c>
       <c r="Q37" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>GOOD</v>
       </c>
       <c r="R37" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>GOOD</v>
       </c>
       <c r="S37">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>14.6</v>
       </c>
       <c r="T37" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>GOOD</v>
       </c>
       <c r="U37">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>8</v>
       </c>
       <c r="V37">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>8</v>
       </c>
       <c r="W37">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>15</v>
       </c>
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>GOOD</v>
       </c>
       <c r="B38">
@@ -5942,82 +6061,82 @@
         <v>357</v>
       </c>
       <c r="D38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>481</v>
       </c>
       <c r="E38" t="s">
         <v>356</v>
       </c>
       <c r="F38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>494</v>
       </c>
       <c r="G38" t="s">
         <v>306</v>
       </c>
       <c r="H38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>550</v>
       </c>
       <c r="I38" t="s">
         <v>307</v>
       </c>
       <c r="J38">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>548</v>
       </c>
       <c r="L38">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>487.5</v>
       </c>
       <c r="M38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>549</v>
       </c>
       <c r="N38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1036.5</v>
       </c>
       <c r="O38" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>Good</v>
       </c>
       <c r="P38" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>GOOD</v>
       </c>
       <c r="Q38" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>GOOD</v>
       </c>
       <c r="R38" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>GOOD</v>
       </c>
       <c r="S38">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>13.82</v>
       </c>
       <c r="T38" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>GOOD</v>
       </c>
       <c r="U38">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>7</v>
       </c>
       <c r="V38">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>8</v>
       </c>
       <c r="W38">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>GOOD</v>
       </c>
       <c r="B39">
@@ -6027,82 +6146,82 @@
         <v>358</v>
       </c>
       <c r="D39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>488</v>
       </c>
       <c r="E39" t="s">
         <v>75</v>
       </c>
       <c r="F39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>486</v>
       </c>
       <c r="G39" t="s">
         <v>277</v>
       </c>
       <c r="H39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>560</v>
       </c>
       <c r="I39" t="s">
         <v>276</v>
       </c>
       <c r="J39">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>559</v>
       </c>
       <c r="L39">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>487</v>
       </c>
       <c r="M39">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>559.5</v>
       </c>
       <c r="N39">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1046.5</v>
       </c>
       <c r="O39" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>Good</v>
       </c>
       <c r="P39" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>BAD</v>
       </c>
       <c r="Q39" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>GOOD</v>
       </c>
       <c r="R39" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>GOOD</v>
       </c>
       <c r="S39">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>13.953333333333333</v>
       </c>
       <c r="T39" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>GOOD</v>
       </c>
       <c r="U39">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>7</v>
       </c>
       <c r="V39">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>8</v>
       </c>
       <c r="W39">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>14</v>
       </c>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>GOOD</v>
       </c>
       <c r="B40">
@@ -6112,82 +6231,82 @@
         <v>85</v>
       </c>
       <c r="D40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>450</v>
       </c>
       <c r="E40" t="s">
         <v>86</v>
       </c>
       <c r="F40">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>443</v>
       </c>
       <c r="G40" t="s">
         <v>309</v>
       </c>
       <c r="H40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>508</v>
       </c>
       <c r="I40" t="s">
         <v>308</v>
       </c>
       <c r="J40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>506</v>
       </c>
       <c r="L40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>446.5</v>
       </c>
       <c r="M40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>507</v>
       </c>
       <c r="N40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>953.5</v>
       </c>
       <c r="O40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>Good</v>
       </c>
       <c r="P40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>GOOD</v>
       </c>
       <c r="Q40" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>GOOD</v>
       </c>
       <c r="R40" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>GOOD</v>
       </c>
       <c r="S40">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>12.713333333333333</v>
       </c>
       <c r="T40" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>GOOD</v>
       </c>
       <c r="U40">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>6</v>
       </c>
       <c r="V40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>7</v>
       </c>
       <c r="W40">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>12</v>
       </c>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>GOOD</v>
       </c>
       <c r="B41">
@@ -6197,82 +6316,82 @@
         <v>269</v>
       </c>
       <c r="D41">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>546</v>
       </c>
       <c r="E41" t="s">
         <v>268</v>
       </c>
       <c r="F41">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>546</v>
       </c>
       <c r="G41" t="s">
         <v>266</v>
       </c>
       <c r="H41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>485</v>
       </c>
       <c r="I41" t="s">
         <v>267</v>
       </c>
       <c r="J41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>490</v>
       </c>
       <c r="L41">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>546</v>
       </c>
       <c r="M41">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>487.5</v>
       </c>
       <c r="N41">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1033.5</v>
       </c>
       <c r="O41" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>Good</v>
       </c>
       <c r="P41" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>GOOD</v>
       </c>
       <c r="Q41" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>GOOD</v>
       </c>
       <c r="R41" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>GOOD</v>
       </c>
       <c r="S41">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>13.78</v>
       </c>
       <c r="T41" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>GOOD</v>
       </c>
       <c r="U41">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>8</v>
       </c>
       <c r="V41">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>7</v>
       </c>
       <c r="W41">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>GOOD</v>
       </c>
       <c r="B42">
@@ -6282,82 +6401,82 @@
         <v>104</v>
       </c>
       <c r="D42">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>443</v>
       </c>
       <c r="E42" t="s">
         <v>105</v>
       </c>
       <c r="F42">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>434</v>
       </c>
       <c r="G42" t="s">
         <v>363</v>
       </c>
       <c r="H42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>472</v>
       </c>
       <c r="I42" t="s">
         <v>362</v>
       </c>
       <c r="J42">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>504</v>
       </c>
       <c r="L42">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>438.5</v>
       </c>
       <c r="M42">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>488</v>
       </c>
       <c r="N42">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>926.5</v>
       </c>
       <c r="O42" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>Good</v>
       </c>
       <c r="P42" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>GOOD</v>
       </c>
       <c r="Q42" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>GOOD</v>
       </c>
       <c r="R42" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>GOOD</v>
       </c>
       <c r="S42">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>12.353333333333333</v>
       </c>
       <c r="T42" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>BAD</v>
       </c>
       <c r="U42">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>6</v>
       </c>
       <c r="V42">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>7</v>
       </c>
       <c r="W42">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>12</v>
       </c>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>GOOD</v>
       </c>
       <c r="B43">
@@ -6367,82 +6486,82 @@
         <v>359</v>
       </c>
       <c r="D43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>478</v>
       </c>
       <c r="E43" t="s">
         <v>115</v>
       </c>
       <c r="F43">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>475</v>
       </c>
       <c r="G43" t="s">
         <v>313</v>
       </c>
       <c r="H43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>560</v>
       </c>
       <c r="I43" t="s">
         <v>312</v>
       </c>
       <c r="J43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>558</v>
       </c>
       <c r="L43">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>476.5</v>
       </c>
       <c r="M43">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>559</v>
       </c>
       <c r="N43">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1035.5</v>
       </c>
       <c r="O43" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>Good</v>
       </c>
       <c r="P43" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>BAD</v>
       </c>
       <c r="Q43" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>GOOD</v>
       </c>
       <c r="R43" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>GOOD</v>
       </c>
       <c r="S43">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>13.806666666666667</v>
       </c>
       <c r="T43" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>GOOD</v>
       </c>
       <c r="U43">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>7</v>
       </c>
       <c r="V43">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>8</v>
       </c>
       <c r="W43">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>14</v>
       </c>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>GOOD</v>
       </c>
       <c r="B44">
@@ -6452,82 +6571,82 @@
         <v>314</v>
       </c>
       <c r="D44">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>532</v>
       </c>
       <c r="E44" t="s">
         <v>315</v>
       </c>
       <c r="F44">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>525</v>
       </c>
       <c r="G44" t="s">
         <v>316</v>
       </c>
       <c r="H44">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>564</v>
       </c>
       <c r="I44" t="s">
         <v>317</v>
       </c>
       <c r="J44">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>567</v>
       </c>
       <c r="L44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>528.5</v>
       </c>
       <c r="M44">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>565.5</v>
       </c>
       <c r="N44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1094</v>
       </c>
       <c r="O44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>Good</v>
       </c>
       <c r="P44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>GOOD</v>
       </c>
       <c r="Q44" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>GOOD</v>
       </c>
       <c r="R44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>GOOD</v>
       </c>
       <c r="S44">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>14.586666666666666</v>
       </c>
       <c r="T44" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>GOOD</v>
       </c>
       <c r="U44">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>8</v>
       </c>
       <c r="V44">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>8</v>
       </c>
       <c r="W44">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>15</v>
       </c>
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>GOOD</v>
       </c>
       <c r="B45">
@@ -6537,82 +6656,82 @@
         <v>134</v>
       </c>
       <c r="D45">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>505</v>
       </c>
       <c r="E45" t="s">
         <v>135</v>
       </c>
       <c r="F45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>507</v>
       </c>
       <c r="G45" t="s">
         <v>318</v>
       </c>
       <c r="H45">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>522</v>
       </c>
       <c r="I45" t="s">
         <v>319</v>
       </c>
       <c r="J45">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>522</v>
       </c>
       <c r="L45">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>506</v>
       </c>
       <c r="M45">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>522</v>
       </c>
       <c r="N45">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1028</v>
       </c>
       <c r="O45" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>Good</v>
       </c>
       <c r="P45" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>GOOD</v>
       </c>
       <c r="Q45" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>GOOD</v>
       </c>
       <c r="R45" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>GOOD</v>
       </c>
       <c r="S45">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>13.706666666666667</v>
       </c>
       <c r="T45" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>GOOD</v>
       </c>
       <c r="U45">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>7</v>
       </c>
       <c r="V45">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>7</v>
       </c>
       <c r="W45">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>13</v>
       </c>
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>GOOD</v>
       </c>
       <c r="B46">
@@ -6622,82 +6741,82 @@
         <v>144</v>
       </c>
       <c r="D46">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>518</v>
       </c>
       <c r="E46" t="s">
         <v>145</v>
       </c>
       <c r="F46">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>533</v>
       </c>
       <c r="G46" t="s">
         <v>146</v>
       </c>
       <c r="H46">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>508</v>
       </c>
       <c r="I46" t="s">
         <v>147</v>
       </c>
       <c r="J46">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>509</v>
       </c>
       <c r="L46">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>525.5</v>
       </c>
       <c r="M46">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>508.5</v>
       </c>
       <c r="N46">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1034</v>
       </c>
       <c r="O46" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>Good</v>
       </c>
       <c r="P46" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>GOOD</v>
       </c>
       <c r="Q46" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>GOOD</v>
       </c>
       <c r="R46" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>GOOD</v>
       </c>
       <c r="S46">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>13.786666666666667</v>
       </c>
       <c r="T46" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>GOOD</v>
       </c>
       <c r="U46">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>8</v>
       </c>
       <c r="V46">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>7</v>
       </c>
       <c r="W46">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>GOOD</v>
       </c>
       <c r="B47">
@@ -6707,82 +6826,82 @@
         <v>155</v>
       </c>
       <c r="D47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>543</v>
       </c>
       <c r="E47" t="s">
         <v>156</v>
       </c>
       <c r="F47">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>538</v>
       </c>
       <c r="G47" t="s">
         <v>279</v>
       </c>
       <c r="H47">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>483</v>
       </c>
       <c r="I47" t="s">
         <v>278</v>
       </c>
       <c r="J47">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>479</v>
       </c>
       <c r="L47">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>540.5</v>
       </c>
       <c r="M47">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>481</v>
       </c>
       <c r="N47">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1021.5</v>
       </c>
       <c r="O47" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>Good</v>
       </c>
       <c r="P47" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>GOOD</v>
       </c>
       <c r="Q47" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>GOOD</v>
       </c>
       <c r="R47" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>GOOD</v>
       </c>
       <c r="S47">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>13.62</v>
       </c>
       <c r="T47" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>GOOD</v>
       </c>
       <c r="U47">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>8</v>
       </c>
       <c r="V47">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>7</v>
       </c>
       <c r="W47">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>14</v>
       </c>
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A48" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>GOOD</v>
       </c>
       <c r="B48">
@@ -6792,82 +6911,82 @@
         <v>321</v>
       </c>
       <c r="D48">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>544</v>
       </c>
       <c r="E48" t="s">
         <v>320</v>
       </c>
       <c r="F48">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>538</v>
       </c>
       <c r="G48" t="s">
         <v>323</v>
       </c>
       <c r="H48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>554</v>
       </c>
       <c r="I48" t="s">
         <v>322</v>
       </c>
       <c r="J48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>552</v>
       </c>
       <c r="L48">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>541</v>
       </c>
       <c r="M48">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>553</v>
       </c>
       <c r="N48">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1094</v>
       </c>
       <c r="O48" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>Good</v>
       </c>
       <c r="P48" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>GOOD</v>
       </c>
       <c r="Q48" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>GOOD</v>
       </c>
       <c r="R48" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>GOOD</v>
       </c>
       <c r="S48">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>14.586666666666666</v>
       </c>
       <c r="T48" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>GOOD</v>
       </c>
       <c r="U48">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>8</v>
       </c>
       <c r="V48">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>8</v>
       </c>
       <c r="W48">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>15</v>
       </c>
     </row>
     <row r="49" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A49" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>GOOD</v>
       </c>
       <c r="B49">
@@ -6877,82 +6996,82 @@
         <v>175</v>
       </c>
       <c r="D49">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>482</v>
       </c>
       <c r="E49" t="s">
         <v>176</v>
       </c>
       <c r="F49">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>481</v>
       </c>
       <c r="G49" t="s">
         <v>325</v>
       </c>
       <c r="H49">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>548</v>
       </c>
       <c r="I49" t="s">
         <v>324</v>
       </c>
       <c r="J49">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>549</v>
       </c>
       <c r="L49">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>481.5</v>
       </c>
       <c r="M49">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>548.5</v>
       </c>
       <c r="N49">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1030</v>
       </c>
       <c r="O49" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>Good</v>
       </c>
       <c r="P49" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>GOOD</v>
       </c>
       <c r="Q49" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>GOOD</v>
       </c>
       <c r="R49" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>GOOD</v>
       </c>
       <c r="S49">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>13.733333333333333</v>
       </c>
       <c r="T49" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>GOOD</v>
       </c>
       <c r="U49">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>7</v>
       </c>
       <c r="V49">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>8</v>
       </c>
       <c r="W49">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>14</v>
       </c>
     </row>
     <row r="50" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>GOOD</v>
       </c>
       <c r="B50">
@@ -6962,82 +7081,82 @@
         <v>331</v>
       </c>
       <c r="D50">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>505</v>
       </c>
       <c r="E50" t="s">
         <v>330</v>
       </c>
       <c r="F50">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>506</v>
       </c>
       <c r="G50" t="s">
         <v>280</v>
       </c>
       <c r="H50">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>568</v>
       </c>
       <c r="I50" t="s">
         <v>281</v>
       </c>
       <c r="J50">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>564</v>
       </c>
       <c r="L50">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>505.5</v>
       </c>
       <c r="M50">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>566</v>
       </c>
       <c r="N50">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1071.5</v>
       </c>
       <c r="O50" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>Good</v>
       </c>
       <c r="P50" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>GOOD</v>
       </c>
       <c r="Q50" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>GOOD</v>
       </c>
       <c r="R50" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>GOOD</v>
       </c>
       <c r="S50">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>14.286666666666667</v>
       </c>
       <c r="T50" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>GOOD</v>
       </c>
       <c r="U50">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>7</v>
       </c>
       <c r="V50">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>8</v>
       </c>
       <c r="W50">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>14</v>
       </c>
     </row>
     <row r="51" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>GOOD</v>
       </c>
       <c r="B51">
@@ -7047,82 +7166,82 @@
         <v>192</v>
       </c>
       <c r="D51">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>522</v>
       </c>
       <c r="E51" t="s">
         <v>193</v>
       </c>
       <c r="F51">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>518</v>
       </c>
       <c r="G51" t="s">
         <v>327</v>
       </c>
       <c r="H51">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>572</v>
       </c>
       <c r="I51" t="s">
         <v>326</v>
       </c>
       <c r="J51">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>572</v>
       </c>
       <c r="L51">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>520</v>
       </c>
       <c r="M51">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>572</v>
       </c>
       <c r="N51">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1092</v>
       </c>
       <c r="O51" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>Good</v>
       </c>
       <c r="P51" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>GOOD</v>
       </c>
       <c r="Q51" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>GOOD</v>
       </c>
       <c r="R51" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>GOOD</v>
       </c>
       <c r="S51">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>14.56</v>
       </c>
       <c r="T51" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>GOOD</v>
       </c>
       <c r="U51">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>7</v>
       </c>
       <c r="V51">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>8</v>
       </c>
       <c r="W51">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>14</v>
       </c>
     </row>
     <row r="52" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>GOOD</v>
       </c>
       <c r="B52">
@@ -7132,82 +7251,82 @@
         <v>201</v>
       </c>
       <c r="D52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>491</v>
       </c>
       <c r="E52" t="s">
         <v>282</v>
       </c>
       <c r="F52">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>492</v>
       </c>
       <c r="G52" t="s">
         <v>328</v>
       </c>
       <c r="H52">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>547</v>
       </c>
       <c r="I52" t="s">
         <v>329</v>
       </c>
       <c r="J52">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>546</v>
       </c>
       <c r="L52">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>491.5</v>
       </c>
       <c r="M52">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>546.5</v>
       </c>
       <c r="N52">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1038</v>
       </c>
       <c r="O52" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>Good</v>
       </c>
       <c r="P52" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>GOOD</v>
       </c>
       <c r="Q52" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>GOOD</v>
       </c>
       <c r="R52" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>GOOD</v>
       </c>
       <c r="S52">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>13.84</v>
       </c>
       <c r="T52" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>GOOD</v>
       </c>
       <c r="U52">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>7</v>
       </c>
       <c r="V52">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>8</v>
       </c>
       <c r="W52">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>14</v>
       </c>
     </row>
     <row r="53" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>GOOD</v>
       </c>
       <c r="B53">
@@ -7217,82 +7336,82 @@
         <v>210</v>
       </c>
       <c r="D53">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>544</v>
       </c>
       <c r="E53" t="s">
         <v>211</v>
       </c>
       <c r="F53">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>530</v>
       </c>
       <c r="G53" t="s">
         <v>332</v>
       </c>
       <c r="H53">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>552</v>
       </c>
       <c r="I53" t="s">
         <v>333</v>
       </c>
       <c r="J53">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>557</v>
       </c>
       <c r="L53">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>537</v>
       </c>
       <c r="M53">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>554.5</v>
       </c>
       <c r="N53">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1091.5</v>
       </c>
       <c r="O53" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>Good</v>
       </c>
       <c r="P53" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>GOOD</v>
       </c>
       <c r="Q53" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>GOOD</v>
       </c>
       <c r="R53" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>GOOD</v>
       </c>
       <c r="S53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>14.553333333333333</v>
       </c>
       <c r="T53" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>GOOD</v>
       </c>
       <c r="U53">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>8</v>
       </c>
       <c r="V53">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>8</v>
       </c>
       <c r="W53">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>15</v>
       </c>
     </row>
     <row r="54" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A54" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>GOOD</v>
       </c>
       <c r="B54">
@@ -7302,82 +7421,82 @@
         <v>221</v>
       </c>
       <c r="D54">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>524</v>
       </c>
       <c r="E54" t="s">
         <v>222</v>
       </c>
       <c r="F54">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>525</v>
       </c>
       <c r="G54" t="s">
         <v>223</v>
       </c>
       <c r="H54">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>574</v>
       </c>
       <c r="I54" t="s">
         <v>224</v>
       </c>
       <c r="J54">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>575</v>
       </c>
       <c r="L54">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>524.5</v>
       </c>
       <c r="M54">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>574.5</v>
       </c>
       <c r="N54">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1099</v>
       </c>
       <c r="O54" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>Good</v>
       </c>
       <c r="P54" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>GOOD</v>
       </c>
       <c r="Q54" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>GOOD</v>
       </c>
       <c r="R54" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>GOOD</v>
       </c>
       <c r="S54">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>14.653333333333334</v>
       </c>
       <c r="T54" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>GOOD</v>
       </c>
       <c r="U54">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>7</v>
       </c>
       <c r="V54">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>8</v>
       </c>
       <c r="W54">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>14</v>
       </c>
     </row>
     <row r="55" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A55" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>GOOD</v>
       </c>
       <c r="B55">
@@ -7387,82 +7506,82 @@
         <v>234</v>
       </c>
       <c r="D55">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>471</v>
       </c>
       <c r="E55" t="s">
         <v>235</v>
       </c>
       <c r="F55">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>468</v>
       </c>
       <c r="G55" t="s">
         <v>335</v>
       </c>
       <c r="H55">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>528</v>
       </c>
       <c r="I55" t="s">
         <v>334</v>
       </c>
       <c r="J55">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>530</v>
       </c>
       <c r="L55">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>469.5</v>
       </c>
       <c r="M55">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>529</v>
       </c>
       <c r="N55">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>998.5</v>
       </c>
       <c r="O55" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>Good</v>
       </c>
       <c r="P55" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>GOOD</v>
       </c>
       <c r="Q55" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>GOOD</v>
       </c>
       <c r="R55" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>GOOD</v>
       </c>
       <c r="S55">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>13.313333333333333</v>
       </c>
       <c r="T55" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>GOOD</v>
       </c>
       <c r="U55">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>7</v>
       </c>
       <c r="V55">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>8</v>
       </c>
       <c r="W55">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>14</v>
       </c>
     </row>
     <row r="56" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A56" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>GOOD</v>
       </c>
       <c r="B56">
@@ -7472,76 +7591,76 @@
         <v>244</v>
       </c>
       <c r="D56">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>475</v>
       </c>
       <c r="E56" t="s">
         <v>244</v>
       </c>
       <c r="F56">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>475</v>
       </c>
       <c r="G56" t="s">
         <v>245</v>
       </c>
       <c r="H56">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>520</v>
       </c>
       <c r="I56" t="s">
         <v>245</v>
       </c>
       <c r="J56">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>520</v>
       </c>
       <c r="L56">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>475</v>
       </c>
       <c r="M56">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>520</v>
       </c>
       <c r="N56">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>995</v>
       </c>
       <c r="O56" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>Good</v>
       </c>
       <c r="P56" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>GOOD</v>
       </c>
       <c r="Q56" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>GOOD</v>
       </c>
       <c r="R56" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>GOOD</v>
       </c>
       <c r="S56">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>13.266666666666667</v>
       </c>
       <c r="T56" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>GOOD</v>
       </c>
       <c r="U56">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>7</v>
       </c>
       <c r="V56">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>7</v>
       </c>
       <c r="W56">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>13</v>
       </c>
     </row>
@@ -15234,7 +15353,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="AA2" sqref="AA2:AA209"/>
     </sheetView>
   </sheetViews>

</xml_diff>